<commit_message>
cập nhật kết quả
</commit_message>
<xml_diff>
--- a/Document/CompResult.xlsx
+++ b/Document/CompResult.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" activeTab="2"/>
@@ -11,7 +11,7 @@
     <sheet name="CompResult" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -637,8 +637,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,25 +772,14 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -810,7 +799,6 @@
               <a:srgbClr val="C00000"/>
             </a:solidFill>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$17:$E$17</c:f>
@@ -872,7 +860,6 @@
               <a:srgbClr val="89E664"/>
             </a:solidFill>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$17:$E$17</c:f>
@@ -915,63 +902,45 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="72790400"/>
-        <c:axId val="72791936"/>
+        <c:axId val="74231808"/>
+        <c:axId val="74233344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="72790400"/>
+        <c:axId val="74231808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72791936"/>
+        <c:crossAx val="74233344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72791936"/>
+        <c:axId val="74233344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72790400"/>
+        <c:crossAx val="74231808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1087,7 +1056,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1122,7 +1090,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1298,21 +1265,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1335,7 +1302,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1358,7 +1325,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1381,7 +1348,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1404,7 +1371,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1427,7 +1394,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1448,7 +1415,7 @@
         <v>0.69000000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1465,7 +1432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1482,7 +1449,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1499,7 +1466,7 @@
         <v>0.51500000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1516,7 +1483,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1533,7 +1500,7 @@
         <v>0.48499999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1554,7 +1521,7 @@
         <v>0.5675</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
         <v>42</v>
@@ -1569,7 +1536,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="9" t="s">
         <v>43</v>
       </c>
@@ -1586,7 +1553,7 @@
         <v>76.75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="9" t="s">
         <v>44</v>
       </c>
@@ -1611,145 +1578,145 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="26.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="138.5703125" style="6" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="26.25" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="26.25" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="26.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="26.25" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="26.25" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="26.25" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="26.25" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="26.25" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="26.25" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="26.25" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="26.25" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="26.25" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="26.25" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="26.25" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="26.25" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="26.25" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="26.25" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="26.25" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="26.25" customHeight="1">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="26.25" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="26.25" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="26.25" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="26.25" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="26.25" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="26.25" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="26.25" customHeight="1">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
@@ -1764,14 +1731,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="9"/>
     <col min="2" max="2" width="10.85546875" style="9" customWidth="1"/>
@@ -1781,7 +1748,7 @@
     <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1795,7 +1762,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="14" t="s">
         <v>57</v>
       </c>
@@ -1804,7 +1771,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="9" t="s">
         <v>45</v>
       </c>
@@ -1818,10 +1785,10 @@
         <v>66</v>
       </c>
       <c r="E3" s="9">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="9" t="s">
         <v>46</v>
       </c>
@@ -1838,7 +1805,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
@@ -1855,7 +1822,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="9" t="s">
         <v>47</v>
       </c>
@@ -1872,7 +1839,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="9" t="s">
         <v>48</v>
       </c>
@@ -1889,7 +1856,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="9" t="s">
         <v>49</v>
       </c>
@@ -1903,10 +1870,10 @@
         <v>81</v>
       </c>
       <c r="E8" s="9">
-        <v>77.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="9" t="s">
         <v>50</v>
       </c>
@@ -1920,10 +1887,10 @@
         <v>88</v>
       </c>
       <c r="E9" s="9">
-        <v>75.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="9" t="s">
         <v>51</v>
       </c>
@@ -1940,7 +1907,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="10" t="s">
         <v>1</v>
       </c>
@@ -1957,7 +1924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="9" t="s">
         <v>52</v>
       </c>
@@ -1971,10 +1938,10 @@
         <v>95</v>
       </c>
       <c r="E12" s="9">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="10" t="s">
         <v>2</v>
       </c>
@@ -1991,7 +1958,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="10" t="s">
         <v>3</v>
       </c>
@@ -2008,7 +1975,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="9" t="s">
         <v>53</v>
       </c>
@@ -2025,7 +1992,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="9" t="s">
         <v>54</v>
       </c>
@@ -2042,7 +2009,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="9" t="s">
         <v>55</v>
       </c>
@@ -2059,7 +2026,7 @@
         <v>90.5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="9" t="s">
         <v>56</v>
       </c>
@@ -2073,10 +2040,10 @@
         <v>41.5</v>
       </c>
       <c r="E18" s="9">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="9" t="s">
         <v>59</v>
       </c>
@@ -2093,7 +2060,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="B20" s="9">
         <f>AVERAGE(B3:B19)</f>
         <v>72.294117647058826</v>
@@ -2108,10 +2075,10 @@
       </c>
       <c r="E20" s="9">
         <f t="shared" si="0"/>
-        <v>74.705882352941174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75.941176470588232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="14" t="s">
         <v>58</v>
       </c>
@@ -2120,7 +2087,7 @@
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="9" t="s">
         <v>45</v>
       </c>
@@ -2137,7 +2104,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="9" t="s">
         <v>46</v>
       </c>
@@ -2154,7 +2121,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -2171,7 +2138,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>47</v>
       </c>
@@ -2188,7 +2155,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>48</v>
       </c>
@@ -2205,7 +2172,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>49</v>
       </c>
@@ -2222,7 +2189,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>50</v>
       </c>
@@ -2239,7 +2206,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>51</v>
       </c>
@@ -2256,7 +2223,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="10" t="s">
         <v>1</v>
       </c>
@@ -2273,7 +2240,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="9" t="s">
         <v>52</v>
       </c>
@@ -2290,7 +2257,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="10" t="s">
         <v>2</v>
       </c>
@@ -2307,7 +2274,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="10" t="s">
         <v>3</v>
       </c>
@@ -2324,7 +2291,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>53</v>
       </c>
@@ -2341,7 +2308,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="9" t="s">
         <v>54</v>
       </c>
@@ -2358,7 +2325,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="9" t="s">
         <v>55</v>
       </c>
@@ -2375,7 +2342,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>56</v>
       </c>
@@ -2392,12 +2359,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="B39" s="9">
         <f>AVERAGE(B22:B38)</f>
         <v>58.03125</v>
@@ -2411,7 +2378,7 @@
         <v>61.71875</v>
       </c>
       <c r="E39" s="9">
-        <f t="shared" ref="B39:E39" si="1">AVERAGE(E22:E38)</f>
+        <f t="shared" ref="E39" si="1">AVERAGE(E22:E38)</f>
         <v>59.8125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Kết quả test DT và chọn tham số Split là Gain Ratio, Prune là Reduced-Error. cập nhật kết quả test DT-ANN
</commit_message>
<xml_diff>
--- a/Document/CompResult.xlsx
+++ b/Document/CompResult.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" activeTab="2"/>
@@ -11,7 +11,7 @@
     <sheet name="CompResult" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -640,8 +640,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -708,24 +708,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -740,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -763,13 +751,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,14 +775,25 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -818,6 +813,7 @@
               <a:srgbClr val="C00000"/>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$17:$E$17</c:f>
@@ -879,6 +875,7 @@
               <a:srgbClr val="89E664"/>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$17:$E$17</c:f>
@@ -921,45 +918,63 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="63675392"/>
-        <c:axId val="63677184"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="69957120"/>
+        <c:axId val="69958656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63675392"/>
+        <c:axId val="69957120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63677184"/>
+        <c:crossAx val="69958656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63677184"/>
+        <c:axId val="69958656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63675392"/>
+        <c:crossAx val="69957120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1075,6 +1090,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1109,6 +1125,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1284,21 +1301,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1321,7 +1338,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1344,7 +1361,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1367,7 +1384,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1390,7 +1407,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1413,7 +1430,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1434,7 +1451,7 @@
         <v>0.69000000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1451,7 +1468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1468,7 +1485,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1485,7 +1502,7 @@
         <v>0.51500000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1502,7 +1519,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1519,7 +1536,7 @@
         <v>0.48499999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1540,7 +1557,7 @@
         <v>0.5675</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
         <v>42</v>
@@ -1555,7 +1572,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>43</v>
       </c>
@@ -1572,7 +1589,7 @@
         <v>76.75</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>44</v>
       </c>
@@ -1597,145 +1614,145 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="26.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="138.5703125" style="6" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="26.25" customHeight="1">
+    <row r="1" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="26.25" customHeight="1">
+    <row r="2" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="26.25" customHeight="1">
+    <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="26.25" customHeight="1">
+    <row r="4" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="26.25" customHeight="1">
+    <row r="5" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="26.25" customHeight="1">
+    <row r="6" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="26.25" customHeight="1">
+    <row r="7" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="26.25" customHeight="1">
+    <row r="8" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="26.25" customHeight="1">
+    <row r="9" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="26.25" customHeight="1">
+    <row r="10" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="26.25" customHeight="1">
+    <row r="11" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="26.25" customHeight="1">
+    <row r="12" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="26.25" customHeight="1">
+    <row r="13" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="26.25" customHeight="1">
+    <row r="14" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="26.25" customHeight="1">
+    <row r="15" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="26.25" customHeight="1">
+    <row r="16" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="26.25" customHeight="1">
+    <row r="17" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="26.25" customHeight="1">
+    <row r="18" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="26.25" customHeight="1">
+    <row r="19" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="26.25" customHeight="1">
+    <row r="20" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="26.25" customHeight="1">
+    <row r="21" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="26.25" customHeight="1">
+    <row r="22" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="26.25" customHeight="1">
+    <row r="23" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="26.25" customHeight="1">
+    <row r="24" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="26.25" customHeight="1">
+    <row r="25" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="26.25" customHeight="1">
+    <row r="26" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
@@ -1750,14 +1767,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="9"/>
     <col min="2" max="2" width="10.85546875" style="9" customWidth="1"/>
@@ -1767,158 +1784,182 @@
     <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="15" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="9">
         <v>73</v>
       </c>
+      <c r="C3" s="9">
+        <v>67.5</v>
+      </c>
       <c r="D3" s="9">
-        <v>67.5</v>
+        <v>66</v>
       </c>
       <c r="E3" s="9">
-        <v>66</v>
-      </c>
-      <c r="F3" s="14">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="9">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="9">
         <v>85.5</v>
       </c>
+      <c r="C4" s="9">
+        <v>65</v>
+      </c>
       <c r="D4" s="9">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="E4" s="9">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F4" s="9">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9">
         <v>68.5</v>
       </c>
+      <c r="C5" s="9">
+        <v>71.5</v>
+      </c>
       <c r="D5" s="9">
-        <v>71.5</v>
-      </c>
-      <c r="E5" s="9">
         <v>73.5</v>
       </c>
-      <c r="F5" s="11">
+      <c r="E5" s="11">
         <v>76.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" s="9">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="9">
         <v>50.5</v>
       </c>
+      <c r="C6" s="9">
+        <v>49</v>
+      </c>
       <c r="D6" s="9">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E6" s="9">
-        <v>54</v>
+        <v>49.5</v>
       </c>
       <c r="F6" s="9">
-        <v>49.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="9">
         <v>57</v>
       </c>
+      <c r="C7" s="9">
+        <v>60</v>
+      </c>
       <c r="D7" s="9">
         <v>60</v>
       </c>
       <c r="E7" s="9">
-        <v>60</v>
+        <v>60.5</v>
       </c>
       <c r="F7" s="9">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>57.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="9">
         <v>83</v>
       </c>
+      <c r="C8" s="9">
+        <v>77.5</v>
+      </c>
       <c r="D8" s="9">
-        <v>77.5</v>
+        <v>81</v>
       </c>
       <c r="E8" s="9">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F8" s="9">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="9">
         <v>85</v>
       </c>
+      <c r="C9" s="9">
+        <v>71.5</v>
+      </c>
       <c r="D9" s="9">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E9" s="9">
-        <v>88</v>
+        <v>85.5</v>
       </c>
       <c r="F9" s="9">
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="9">
         <v>71</v>
       </c>
+      <c r="C10" s="9">
+        <v>65</v>
+      </c>
       <c r="D10" s="9">
         <v>65</v>
       </c>
@@ -1926,84 +1967,99 @@
         <v>65</v>
       </c>
       <c r="F10" s="9">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="9">
         <v>59.5</v>
       </c>
+      <c r="C11" s="9">
+        <v>63.5</v>
+      </c>
       <c r="D11" s="9">
-        <v>63.5</v>
+        <v>66.5</v>
       </c>
       <c r="E11" s="9">
-        <v>66.5</v>
+        <v>70</v>
       </c>
       <c r="F11" s="9">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="9">
         <v>75</v>
       </c>
+      <c r="C12" s="9">
+        <v>94.5</v>
+      </c>
       <c r="D12" s="9">
-        <v>94.5</v>
+        <v>95</v>
       </c>
       <c r="E12" s="9">
-        <v>95</v>
+        <v>95.5</v>
       </c>
       <c r="F12" s="9">
-        <v>95.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="9">
         <v>73.5</v>
       </c>
+      <c r="C13" s="9">
+        <v>85</v>
+      </c>
       <c r="D13" s="9">
+        <v>85.5</v>
+      </c>
+      <c r="E13" s="9">
         <v>85</v>
       </c>
-      <c r="E13" s="9">
-        <v>85.5</v>
-      </c>
       <c r="F13" s="9">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>84.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="9">
         <v>74.5</v>
       </c>
+      <c r="C14" s="9">
+        <v>65.5</v>
+      </c>
       <c r="D14" s="9">
-        <v>65.5</v>
-      </c>
-      <c r="E14" s="9">
         <v>71.5</v>
       </c>
-      <c r="F14" s="11">
+      <c r="E14" s="11">
         <v>75.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="F14" s="9">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B15" s="9">
         <v>60.5</v>
       </c>
+      <c r="C15" s="9">
+        <v>60.5</v>
+      </c>
       <c r="D15" s="9">
         <v>60.5</v>
       </c>
@@ -2014,402 +2070,462 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B16" s="9">
         <v>67.5</v>
       </c>
+      <c r="C16" s="9">
+        <v>71.5</v>
+      </c>
       <c r="D16" s="9">
-        <v>71.5</v>
+        <v>84</v>
       </c>
       <c r="E16" s="9">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F16" s="9">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B17" s="9">
         <v>86.5</v>
       </c>
+      <c r="C17" s="9">
+        <v>89.5</v>
+      </c>
       <c r="D17" s="9">
-        <v>89.5</v>
+        <v>90</v>
       </c>
       <c r="E17" s="9">
-        <v>90</v>
+        <v>90.5</v>
       </c>
       <c r="F17" s="9">
-        <v>90.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>86.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B18" s="9">
         <v>70</v>
       </c>
+      <c r="C18" s="9">
+        <v>50</v>
+      </c>
       <c r="D18" s="9">
-        <v>50</v>
+        <v>41.5</v>
       </c>
       <c r="E18" s="9">
-        <v>41.5</v>
+        <v>67</v>
       </c>
       <c r="F18" s="9">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B19" s="9">
         <v>88.5</v>
       </c>
+      <c r="C19" s="9">
+        <v>90</v>
+      </c>
       <c r="D19" s="9">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E19" s="9">
         <v>88</v>
       </c>
       <c r="F19" s="9">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="9">
         <f>AVERAGE(B3:B19)</f>
         <v>72.294117647058826</v>
       </c>
-      <c r="C20" s="9" t="e">
-        <f>AVERAGE(C3:C19)</f>
-        <v>#DIV/0!</v>
+      <c r="C20" s="9">
+        <f t="shared" ref="C20:F20" si="0">AVERAGE(C3:C19)</f>
+        <v>70.411764705882348</v>
       </c>
       <c r="D20" s="9">
-        <f>AVERAGE(D3:D19)</f>
-        <v>71.382352941176464</v>
+        <f t="shared" si="0"/>
+        <v>74.294117647058826</v>
       </c>
       <c r="E20" s="9">
-        <f>AVERAGE(E3:E19)</f>
-        <v>74.294117647058826</v>
+        <f t="shared" si="0"/>
+        <v>75.941176470588232</v>
       </c>
       <c r="F20" s="9">
-        <f>AVERAGE(F3:F19)</f>
-        <v>75.941176470588232</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="15" t="s">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="13">
         <v>77</v>
       </c>
-      <c r="D22" s="18">
+      <c r="C22" s="13">
         <v>66.5</v>
       </c>
-      <c r="E22" s="18">
+      <c r="D22" s="13">
         <v>64.5</v>
       </c>
-      <c r="F22" s="18">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="E22" s="13">
+        <v>59</v>
+      </c>
+      <c r="F22" s="9">
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="13">
         <v>56.5</v>
       </c>
+      <c r="C23" s="13">
+        <v>89</v>
+      </c>
       <c r="D23" s="13">
-        <v>88.5</v>
+        <v>86.5</v>
       </c>
       <c r="E23" s="13">
-        <v>89</v>
-      </c>
-      <c r="F23" s="13">
-        <v>90.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>69.5</v>
+      </c>
+      <c r="F23" s="9">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="9">
         <v>56</v>
       </c>
+      <c r="C24" s="9">
+        <v>57</v>
+      </c>
       <c r="D24" s="9">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E24" s="9">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F24" s="9">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B25" s="9">
         <v>67</v>
       </c>
+      <c r="C25" s="9">
+        <v>18</v>
+      </c>
       <c r="D25" s="9">
-        <v>18</v>
+        <v>24.5</v>
       </c>
       <c r="E25" s="9">
-        <v>24.5</v>
+        <v>21</v>
       </c>
       <c r="F25" s="9">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="9">
         <v>39</v>
       </c>
+      <c r="C26" s="9">
+        <v>60</v>
+      </c>
       <c r="D26" s="9">
-        <v>60</v>
+        <v>59.5</v>
       </c>
       <c r="E26" s="9">
-        <v>59.5</v>
+        <v>60.5</v>
       </c>
       <c r="F26" s="9">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="9">
         <v>34.5</v>
       </c>
+      <c r="C27" s="9">
+        <v>69</v>
+      </c>
       <c r="D27" s="9">
-        <v>69</v>
+        <v>67.5</v>
       </c>
       <c r="E27" s="9">
-        <v>67.5</v>
+        <v>68</v>
       </c>
       <c r="F27" s="9">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B28" s="9">
         <v>76</v>
       </c>
-      <c r="D28" s="14">
+      <c r="C28" s="9">
         <v>61</v>
       </c>
-      <c r="E28" s="14">
+      <c r="D28" s="9">
         <v>65</v>
       </c>
-      <c r="F28" s="14">
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="E28" s="9">
+        <v>61</v>
+      </c>
+      <c r="F28" s="9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="9">
         <v>63.5</v>
       </c>
+      <c r="C29" s="9">
+        <v>65.5</v>
+      </c>
       <c r="D29" s="9">
-        <v>65.5</v>
+        <v>66.5</v>
       </c>
       <c r="E29" s="9">
-        <v>66.5</v>
+        <v>54</v>
       </c>
       <c r="F29" s="9">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="9">
         <v>51.5</v>
       </c>
+      <c r="C30" s="9">
+        <v>64</v>
+      </c>
       <c r="D30" s="9">
-        <v>64</v>
-      </c>
-      <c r="E30" s="9">
         <v>67</v>
       </c>
-      <c r="F30" s="12">
+      <c r="E30" s="12">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="F30" s="9">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B31" s="9">
         <v>33</v>
       </c>
+      <c r="C31" s="9">
+        <v>86.5</v>
+      </c>
       <c r="D31" s="9">
-        <v>86.5</v>
-      </c>
-      <c r="E31" s="9">
         <v>78.5</v>
       </c>
-      <c r="F31" s="12">
+      <c r="E31" s="12">
         <v>87.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="F31" s="9">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="9">
         <v>71</v>
       </c>
+      <c r="C32" s="9">
+        <v>70.5</v>
+      </c>
       <c r="D32" s="9">
-        <v>70.5</v>
-      </c>
-      <c r="E32" s="9">
         <v>74.5</v>
       </c>
-      <c r="F32" s="12">
+      <c r="E32" s="12">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="F32" s="9">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B33" s="9">
         <v>48.5</v>
       </c>
+      <c r="C33" s="9">
+        <v>51.5</v>
+      </c>
       <c r="D33" s="9">
-        <v>51.5</v>
+        <v>56</v>
       </c>
       <c r="E33" s="9">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F33" s="9">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B34" s="9">
         <v>60.5</v>
       </c>
+      <c r="C34" s="9">
+        <v>59.5</v>
+      </c>
       <c r="D34" s="9">
-        <v>59.5</v>
-      </c>
-      <c r="E34" s="9">
         <v>61.5</v>
       </c>
-      <c r="F34" s="12">
+      <c r="E34" s="12">
         <v>56.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="F34" s="9">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B35" s="9">
         <v>54</v>
       </c>
+      <c r="C35" s="9">
+        <v>64</v>
+      </c>
       <c r="D35" s="9">
-        <v>64</v>
-      </c>
-      <c r="E35" s="14">
-        <v>63.5</v>
-      </c>
-      <c r="F35" s="16">
-        <v>68.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>55.5</v>
+      </c>
+      <c r="E35" s="12">
+        <v>57</v>
+      </c>
+      <c r="F35" s="9">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B36" s="9">
         <v>73</v>
       </c>
-      <c r="D36" s="14">
+      <c r="C36" s="9">
         <v>67.5</v>
       </c>
-      <c r="E36" s="14">
+      <c r="D36" s="9">
         <v>69.5</v>
       </c>
-      <c r="F36" s="17">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="E36" s="12">
+        <v>60</v>
+      </c>
+      <c r="F36" s="9">
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="9">
         <v>67.5</v>
       </c>
+      <c r="C37" s="9">
+        <v>15</v>
+      </c>
       <c r="D37" s="9">
-        <v>15</v>
-      </c>
-      <c r="E37" s="9">
         <v>32</v>
       </c>
-      <c r="F37" s="12">
+      <c r="E37" s="12">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="F37" s="9">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="9">
         <f>AVERAGE(B22:B38)</f>
         <v>58.03125</v>
       </c>
-      <c r="C39" s="9" t="e">
+      <c r="C39" s="9">
         <f>AVERAGE(C22:C38)</f>
-        <v>#DIV/0!</v>
+        <v>60.28125</v>
       </c>
       <c r="D39" s="9">
         <f>AVERAGE(D22:D38)</f>
-        <v>60.25</v>
+        <v>61.71875</v>
       </c>
       <c r="E39" s="9">
-        <f>AVERAGE(E22:E38)</f>
-        <v>62.375</v>
+        <f t="shared" ref="E39:F39" si="1">AVERAGE(E22:E38)</f>
+        <v>59.8125</v>
       </c>
       <c r="F39" s="9">
-        <f t="shared" ref="F39" si="0">AVERAGE(F22:F38)</f>
-        <v>65.0625</v>
+        <f t="shared" si="1"/>
+        <v>58.875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bản paper hoàn tất
</commit_message>
<xml_diff>
--- a/Document/CompResult.xlsx
+++ b/Document/CompResult.xlsx
@@ -796,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -834,13 +834,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -898,6 +897,10 @@
               <a:srgbClr val="C00000"/>
             </a:solidFill>
           </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$17:$E$17</c:f>
@@ -922,19 +925,19 @@
             <c:numRef>
               <c:f>Sheet1!$B$18:$E$18</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>69</c:v>
+                  <c:v>73.083333333333329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.375</c:v>
+                  <c:v>74.416666666666671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.25</c:v>
+                  <c:v>76.583333333333329</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.75</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -956,9 +959,16 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="89E664"/>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
             </a:solidFill>
           </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$B$17:$E$17</c:f>
@@ -986,47 +996,47 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>56.75</c:v>
+                  <c:v>54.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60.75</c:v>
+                  <c:v>61.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.13</c:v>
+                  <c:v>63.58</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67.5</c:v>
+                  <c:v>66.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="61005824"/>
-        <c:axId val="61007360"/>
+        <c:axId val="39710080"/>
+        <c:axId val="39711872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61005824"/>
+        <c:axId val="39710080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61007360"/>
+        <c:crossAx val="39711872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61007360"/>
+        <c:axId val="39711872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61005824"/>
+        <c:crossAx val="39710080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1039,7 +1049,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1367,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1639,17 +1649,17 @@
       <c r="A18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="9">
-        <v>69</v>
-      </c>
-      <c r="C18" s="9">
-        <v>71.375</v>
-      </c>
-      <c r="D18" s="9">
-        <v>74.25</v>
-      </c>
-      <c r="E18" s="9">
-        <v>76.75</v>
+      <c r="B18" s="29">
+        <v>73.083333333333329</v>
+      </c>
+      <c r="C18" s="3">
+        <v>74.416666666666671</v>
+      </c>
+      <c r="D18" s="3">
+        <v>76.583333333333329</v>
+      </c>
+      <c r="E18" s="3">
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1657,16 +1667,16 @@
         <v>44</v>
       </c>
       <c r="B19" s="9">
-        <v>56.75</v>
+        <v>54.17</v>
       </c>
       <c r="C19" s="9">
-        <v>60.75</v>
+        <v>61.5</v>
       </c>
       <c r="D19" s="9">
-        <v>64.13</v>
+        <v>63.58</v>
       </c>
       <c r="E19" s="9">
-        <v>67.5</v>
+        <v>66.5</v>
       </c>
     </row>
   </sheetData>
@@ -1849,28 +1859,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="H2" s="32" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="H2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="N2" s="32" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="N2" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="9" t="s">
@@ -1920,14 +1930,14 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="9" t="s">
@@ -2272,14 +2282,14 @@
       </c>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="9" t="s">
@@ -2625,8 +2635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2644,28 +2654,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="H2" s="33" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="H2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="N2" s="33" t="s">
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="N2" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="18" t="s">
@@ -2715,14 +2725,14 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="18" t="s">
@@ -3307,127 +3317,127 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="27" customFormat="1">
-      <c r="B16" s="27">
+    <row r="16" spans="1:18" s="25" customFormat="1">
+      <c r="B16" s="25">
         <f>AVERAGE(B5:B15)</f>
         <v>74.63636363636364</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="25">
         <f>AVERAGE(C5:C15)</f>
         <v>77.727272727272734</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="25">
         <f>AVERAGE(D5:D15)</f>
         <v>77.227272727272734</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="25">
         <f>AVERAGE(E5:E15)</f>
         <v>78.63636363636364</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="25">
         <f>AVERAGE(F5:F15)</f>
         <v>80.318181818181813</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16" s="25">
         <f>AVERAGE(H5:H15)</f>
         <v>78.318181818181813</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="25">
         <f>AVERAGE(I5:I15)</f>
         <v>77.954545454545453</v>
       </c>
-      <c r="J16" s="27">
+      <c r="J16" s="25">
         <f>AVERAGE(J5:J15)</f>
         <v>79.5</v>
       </c>
-      <c r="K16" s="27">
+      <c r="K16" s="25">
         <f>AVERAGE(K5:K15)</f>
         <v>79.818181818181813</v>
       </c>
-      <c r="L16" s="27">
+      <c r="L16" s="25">
         <f>AVERAGE(L5:L15)</f>
         <v>82.045454545454547</v>
       </c>
-      <c r="N16" s="27">
+      <c r="N16" s="25">
         <f>AVERAGE(N5:N15)</f>
         <v>78.045454545454547</v>
       </c>
-      <c r="O16" s="27">
+      <c r="O16" s="25">
         <f>AVERAGE(O5:O15)</f>
         <v>78.5</v>
       </c>
-      <c r="P16" s="27">
+      <c r="P16" s="25">
         <f>AVERAGE(P5:P15)</f>
         <v>79.63636363636364</v>
       </c>
-      <c r="Q16" s="27">
+      <c r="Q16" s="25">
         <f>AVERAGE(Q5:Q15)</f>
         <v>80.5</v>
       </c>
-      <c r="R16" s="27">
+      <c r="R16" s="25">
         <f>AVERAGE(R5:R15)</f>
         <v>82.13636363636364</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="26"/>
-      <c r="B17" s="25">
+    <row r="17" spans="1:18" s="28" customFormat="1">
+      <c r="A17" s="30"/>
+      <c r="B17" s="29">
         <f t="shared" ref="B17:E17" si="0" xml:space="preserve"> (B6+B8+B9+B7+B12+B13)/6</f>
         <v>73.083333333333329</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="29">
         <f t="shared" si="0"/>
         <v>75.25</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="29">
         <f t="shared" si="0"/>
         <v>74.416666666666671</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="29">
         <f t="shared" si="0"/>
         <v>76.583333333333329</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="29">
         <f xml:space="preserve"> (F6+F8+F9+F7+F12+F13)/6</f>
         <v>78</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="29">
         <f t="shared" ref="H17:K17" si="1" xml:space="preserve"> (H6+H8+H9+H7+H12+H13)/6</f>
         <v>76.583333333333329</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="29">
         <f t="shared" si="1"/>
         <v>74.333333333333329</v>
       </c>
-      <c r="J17" s="25">
+      <c r="J17" s="29">
         <f t="shared" si="1"/>
         <v>79.416666666666671</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="29">
         <f t="shared" si="1"/>
         <v>79.083333333333329</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="29">
         <f xml:space="preserve"> (L6+L8+L9+L7+L12+L13)/6</f>
         <v>82</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="29">
         <f t="shared" ref="N17:Q17" si="2" xml:space="preserve"> (N6+N8+N9+N7+N12+N13)/6</f>
         <v>77.333333333333329</v>
       </c>
-      <c r="O17" s="25">
+      <c r="O17" s="29">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="P17" s="25">
+      <c r="P17" s="29">
         <f t="shared" si="2"/>
         <v>79.083333333333329</v>
       </c>
-      <c r="Q17" s="25">
+      <c r="Q17" s="29">
         <f t="shared" si="2"/>
         <v>79.833333333333329</v>
       </c>
-      <c r="R17" s="25">
+      <c r="R17" s="29">
         <f xml:space="preserve"> (R6+R8+R9+R7+R12+R13)/6</f>
         <v>82.25</v>
       </c>
@@ -4015,128 +4025,128 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:18" s="27" customFormat="1">
-      <c r="B29" s="27">
+    <row r="29" spans="1:18" s="25" customFormat="1">
+      <c r="B29" s="25">
         <f>AVERAGE(B18:B28)</f>
         <v>57.954545454545453</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C29" s="25">
         <f>AVERAGE(C18:C28)</f>
         <v>63.636363636363633</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="25">
         <f>AVERAGE(D18:D28)</f>
         <v>66.545454545454547</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="25">
         <f>AVERAGE(E18:E28)</f>
         <v>67.090909090909093</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="25">
         <f>AVERAGE(F18:F28)</f>
         <v>70.545454545454547</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="25">
         <f>AVERAGE(H18:H28)</f>
         <v>69.409090909090907</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="25">
         <f>AVERAGE(I18:I28)</f>
         <v>70.13636363636364</v>
       </c>
-      <c r="J29" s="27">
+      <c r="J29" s="25">
         <f>AVERAGE(J18:J28)</f>
         <v>70.181818181818187</v>
       </c>
-      <c r="K29" s="27">
+      <c r="K29" s="25">
         <f>AVERAGE(K18:K28)</f>
         <v>73.727272727272734</v>
       </c>
-      <c r="L29" s="27">
+      <c r="L29" s="25">
         <f>AVERAGE(L18:L28)</f>
         <v>76</v>
       </c>
-      <c r="N29" s="27">
+      <c r="N29" s="25">
         <f>AVERAGE(N18:N28)</f>
         <v>69.954545454545453</v>
       </c>
-      <c r="O29" s="27">
+      <c r="O29" s="25">
         <f>AVERAGE(O18:O28)</f>
         <v>70.409090909090907</v>
       </c>
-      <c r="P29" s="27">
+      <c r="P29" s="25">
         <f>AVERAGE(P18:P28)</f>
         <v>72.818181818181813</v>
       </c>
-      <c r="Q29" s="27">
+      <c r="Q29" s="25">
         <f>AVERAGE(Q18:Q28)</f>
         <v>74.5</v>
       </c>
-      <c r="R29" s="27">
+      <c r="R29" s="25">
         <f>AVERAGE(R18:R28)</f>
         <v>76.36363636363636</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="30" customFormat="1">
-      <c r="B30" s="31">
+    <row r="30" spans="1:18" s="28" customFormat="1">
+      <c r="B30" s="29">
         <f t="shared" ref="B30:F30" si="3" xml:space="preserve"> (B19+B21+B22+B20+B25+B26)/6</f>
         <v>54.166666666666664</v>
       </c>
-      <c r="C30" s="31">
+      <c r="C30" s="29">
         <f t="shared" si="3"/>
         <v>55.5</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="29">
         <f t="shared" si="3"/>
         <v>61.5</v>
       </c>
-      <c r="E30" s="31">
+      <c r="E30" s="29">
         <f t="shared" si="3"/>
         <v>63.583333333333336</v>
       </c>
-      <c r="F30" s="31">
+      <c r="F30" s="29">
         <f t="shared" si="3"/>
         <v>66.5</v>
       </c>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31">
+      <c r="G30" s="29"/>
+      <c r="H30" s="29">
         <f t="shared" ref="H30:K30" si="4" xml:space="preserve"> (H19+H21+H22+H20+H25+H26)/6</f>
         <v>68.916666666666671</v>
       </c>
-      <c r="I30" s="31">
+      <c r="I30" s="29">
         <f t="shared" si="4"/>
         <v>68.083333333333329</v>
       </c>
-      <c r="J30" s="31">
+      <c r="J30" s="29">
         <f t="shared" si="4"/>
         <v>69.083333333333329</v>
       </c>
-      <c r="K30" s="31">
+      <c r="K30" s="29">
         <f t="shared" si="4"/>
         <v>71.75</v>
       </c>
-      <c r="L30" s="31">
+      <c r="L30" s="29">
         <f xml:space="preserve"> (L19+L21+L22+L20+L25+L26)/6</f>
         <v>73.166666666666671</v>
       </c>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31">
+      <c r="M30" s="29"/>
+      <c r="N30" s="29">
         <f t="shared" ref="N30:R30" si="5" xml:space="preserve"> (N19+N21+N22+N20+N25+N26)/6</f>
         <v>68.666666666666671</v>
       </c>
-      <c r="O30" s="31">
+      <c r="O30" s="29">
         <f t="shared" si="5"/>
         <v>70.25</v>
       </c>
-      <c r="P30" s="31">
+      <c r="P30" s="29">
         <f t="shared" si="5"/>
         <v>70.75</v>
       </c>
-      <c r="Q30" s="31">
+      <c r="Q30" s="29">
         <f t="shared" si="5"/>
         <v>74.833333333333329</v>
       </c>
-      <c r="R30" s="31">
+      <c r="R30" s="29">
         <f t="shared" si="5"/>
         <v>73.25</v>
       </c>
@@ -4155,10 +4165,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:R29"/>
+  <dimension ref="A2:R31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20:F22"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4175,28 +4185,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="H2" s="34" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="N2" s="34" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="20" t="s">
@@ -4246,14 +4256,14 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1">
       <c r="A5" s="20" t="s">
@@ -4711,7 +4721,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1">
@@ -4816,135 +4826,131 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="28" customFormat="1">
-      <c r="B16" s="28">
+    <row r="16" spans="1:18" s="26" customFormat="1">
+      <c r="B16" s="26">
         <f t="shared" ref="B16:L16" si="0">AVERAGE(B5:B15)</f>
         <v>0.72727272727272729</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="26">
         <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="26">
         <f t="shared" si="0"/>
         <v>0.68181818181818177</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="26">
         <f t="shared" si="0"/>
         <v>0.22727272727272727</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="26">
         <f t="shared" si="0"/>
         <v>0.13636363636363635</v>
       </c>
-      <c r="G16" s="28" t="e">
+      <c r="G16" s="26" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="26">
         <f t="shared" si="0"/>
         <v>0.36363636363636365</v>
       </c>
-      <c r="I16" s="28">
+      <c r="I16" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="26">
         <f t="shared" si="0"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="K16" s="28">
+      <c r="K16" s="26">
         <f t="shared" si="0"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="L16" s="28">
+      <c r="L16" s="26">
         <f t="shared" si="0"/>
         <v>4.5454545454545456E-2</v>
       </c>
-      <c r="N16" s="28">
+      <c r="N16" s="26">
         <f>AVERAGE(N5:N15)</f>
         <v>0.36363636363636365</v>
       </c>
-      <c r="O16" s="28">
+      <c r="O16" s="26">
         <f>AVERAGE(O5:O15)</f>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="P16" s="28">
+      <c r="P16" s="26">
         <f>AVERAGE(P5:P15)</f>
         <v>0.63636363636363635</v>
       </c>
-      <c r="Q16" s="28">
+      <c r="Q16" s="26">
         <f>AVERAGE(Q5:Q15)</f>
         <v>0.31818181818181818</v>
       </c>
-      <c r="R16" s="28">
+      <c r="R16" s="26">
         <f>AVERAGE(R5:R15)</f>
-        <v>0.18181818181818182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="34" t="s">
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="26" customFormat="1">
+      <c r="B17" s="29">
+        <f t="shared" ref="B17:L17" si="1" xml:space="preserve"> (B6+B8+B9+B7+B12+B13)/6</f>
+        <v>1.25</v>
+      </c>
+      <c r="C17" s="29">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D17" s="29">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="E17" s="29">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F17" s="29">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="H17" s="29">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="29">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K17" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="29">
+        <f t="shared" ref="R17" si="2" xml:space="preserve"> (R6+R8+R9+R7+R12+R13)/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-    </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="19">
-        <v>0</v>
-      </c>
-      <c r="C18" s="20">
-        <v>0</v>
-      </c>
-      <c r="D18" s="22">
-        <v>0</v>
-      </c>
-      <c r="E18" s="22">
-        <v>2.5</v>
-      </c>
-      <c r="F18" s="22">
-        <v>5</v>
-      </c>
-      <c r="H18" s="9">
-        <v>0</v>
-      </c>
-      <c r="I18" s="9">
-        <v>0</v>
-      </c>
-      <c r="J18" s="20">
-        <v>0</v>
-      </c>
-      <c r="K18" s="20">
-        <v>0</v>
-      </c>
-      <c r="L18" s="9">
-        <v>0</v>
-      </c>
-      <c r="N18" s="9">
-        <v>0</v>
-      </c>
-      <c r="O18" s="9">
-        <v>0</v>
-      </c>
-      <c r="P18" s="20">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="20">
-        <v>0</v>
-      </c>
-      <c r="R18" s="20">
-        <v>1</v>
-      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="20" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B19" s="19">
         <v>0</v>
@@ -4952,14 +4958,14 @@
       <c r="C19" s="20">
         <v>0</v>
       </c>
-      <c r="D19" s="20">
-        <v>0</v>
-      </c>
-      <c r="E19" s="20">
-        <v>0</v>
-      </c>
-      <c r="F19" s="20">
-        <v>0</v>
+      <c r="D19" s="22">
+        <v>0</v>
+      </c>
+      <c r="E19" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="F19" s="22">
+        <v>5</v>
       </c>
       <c r="H19" s="9">
         <v>0</v>
@@ -4989,104 +4995,104 @@
         <v>0</v>
       </c>
       <c r="R19" s="20">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="20">
-        <v>21.5</v>
+        <v>0</v>
+      </c>
+      <c r="B20" s="19">
+        <v>0</v>
       </c>
       <c r="C20" s="20">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D20" s="20">
         <v>0</v>
       </c>
       <c r="E20" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="20">
         <v>0</v>
       </c>
       <c r="H20" s="9">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="I20" s="9">
+        <v>0</v>
+      </c>
+      <c r="J20" s="20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="9">
+        <v>0</v>
+      </c>
+      <c r="N20" s="9">
+        <v>0</v>
+      </c>
+      <c r="O20" s="9">
+        <v>0</v>
+      </c>
+      <c r="P20" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="20">
+        <v>0</v>
+      </c>
+      <c r="R20" s="20">
         <v>0.5</v>
-      </c>
-      <c r="J20" s="20">
-        <v>2.5</v>
-      </c>
-      <c r="K20" s="20">
-        <v>2</v>
-      </c>
-      <c r="L20" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="N20" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="O20" s="9">
-        <v>2</v>
-      </c>
-      <c r="P20" s="20">
-        <v>1.5</v>
-      </c>
-      <c r="Q20" s="20">
-        <v>1.5</v>
-      </c>
-      <c r="R20" s="20">
-        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="20">
-        <v>0</v>
+        <v>21.5</v>
       </c>
       <c r="C21" s="20">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D21" s="20">
         <v>0</v>
       </c>
       <c r="E21" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="20">
         <v>0</v>
       </c>
       <c r="H21" s="9">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I21" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J21" s="20">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="K21" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L21" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N21" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O21" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P21" s="20">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="Q21" s="20">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="R21" s="20">
         <v>0</v>
@@ -5094,7 +5100,7 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="20">
         <v>0</v>
@@ -5102,13 +5108,13 @@
       <c r="C22" s="20">
         <v>0</v>
       </c>
-      <c r="D22" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="E22" s="21">
-        <v>0</v>
-      </c>
-      <c r="F22" s="21">
+      <c r="D22" s="20">
+        <v>0</v>
+      </c>
+      <c r="E22" s="20">
+        <v>0</v>
+      </c>
+      <c r="F22" s="20">
         <v>0</v>
       </c>
       <c r="H22" s="9">
@@ -5118,10 +5124,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="20">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K22" s="20">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L22" s="9">
         <v>0</v>
@@ -5133,10 +5139,10 @@
         <v>0</v>
       </c>
       <c r="P22" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R22" s="20">
         <v>0</v>
@@ -5144,60 +5150,60 @@
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="20">
+        <v>0</v>
+      </c>
+      <c r="C23" s="20">
+        <v>0</v>
+      </c>
+      <c r="D23" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="21">
+        <v>0</v>
+      </c>
+      <c r="F23" s="21">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0</v>
+      </c>
+      <c r="J23" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K23" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="L23" s="9">
+        <v>0</v>
+      </c>
+      <c r="N23" s="9">
+        <v>0</v>
+      </c>
+      <c r="O23" s="9">
+        <v>0</v>
+      </c>
+      <c r="P23" s="20">
         <v>1</v>
       </c>
-      <c r="B23" s="20">
-        <v>4.5</v>
-      </c>
-      <c r="C23" s="20">
-        <v>0</v>
-      </c>
-      <c r="D23" s="20">
-        <v>0</v>
-      </c>
-      <c r="E23" s="20">
-        <v>0</v>
-      </c>
-      <c r="F23" s="20">
-        <v>0</v>
-      </c>
-      <c r="H23" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="I23" s="9">
-        <v>3</v>
-      </c>
-      <c r="J23" s="20">
-        <v>0</v>
-      </c>
-      <c r="K23" s="20">
-        <v>2</v>
-      </c>
-      <c r="L23" s="9">
-        <v>0</v>
-      </c>
-      <c r="N23" s="9">
-        <v>3</v>
-      </c>
-      <c r="O23" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="P23" s="20">
-        <v>2.5</v>
-      </c>
       <c r="Q23" s="20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R23" s="20">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="20" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="B24" s="20">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="C24" s="20">
         <v>0</v>
@@ -5212,45 +5218,45 @@
         <v>0</v>
       </c>
       <c r="H24" s="9">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="I24" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J24" s="20">
         <v>0</v>
       </c>
       <c r="K24" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L24" s="9">
         <v>0</v>
       </c>
       <c r="N24" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O24" s="9">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="P24" s="20">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Q24" s="20">
         <v>0</v>
       </c>
       <c r="R24" s="20">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="20" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B25" s="20">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="C25" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="20">
         <v>0</v>
@@ -5277,7 +5283,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O25" s="9">
         <v>0</v>
@@ -5294,43 +5300,43 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26" s="20">
-        <v>22.5</v>
+        <v>4.5</v>
       </c>
       <c r="C26" s="20">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D26" s="20">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E26" s="20">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F26" s="20">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H26" s="9">
         <v>0</v>
       </c>
       <c r="I26" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="20">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="K26" s="20">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="L26" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26" s="9">
-        <v>4.5</v>
+        <v>0.5</v>
       </c>
       <c r="O26" s="9">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="P26" s="20">
         <v>0</v>
@@ -5339,48 +5345,48 @@
         <v>0</v>
       </c>
       <c r="R26" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="20" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="B27" s="20">
-        <v>0</v>
+        <v>22.5</v>
       </c>
       <c r="C27" s="20">
-        <v>0</v>
-      </c>
-      <c r="D27" s="21">
-        <v>0</v>
-      </c>
-      <c r="E27" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="F27" s="18">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="D27" s="20">
+        <v>21</v>
+      </c>
+      <c r="E27" s="20">
+        <v>18</v>
+      </c>
+      <c r="F27" s="20">
+        <v>13</v>
       </c>
       <c r="H27" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I27" s="9">
         <v>1</v>
       </c>
       <c r="J27" s="20">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="K27" s="20">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="L27" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N27" s="9">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="O27" s="9">
-        <v>0.5</v>
+        <v>3.5</v>
       </c>
       <c r="P27" s="20">
         <v>0</v>
@@ -5389,119 +5395,231 @@
         <v>0</v>
       </c>
       <c r="R27" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="20">
+        <v>0</v>
+      </c>
+      <c r="C28" s="20">
+        <v>0</v>
+      </c>
+      <c r="D28" s="21">
+        <v>0</v>
+      </c>
+      <c r="E28" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="18">
+        <v>0</v>
+      </c>
+      <c r="H28" s="9">
+        <v>3</v>
+      </c>
+      <c r="I28" s="9">
+        <v>1</v>
+      </c>
+      <c r="J28" s="20">
+        <v>6</v>
+      </c>
+      <c r="K28" s="20">
+        <v>2</v>
+      </c>
+      <c r="L28" s="9">
+        <v>2</v>
+      </c>
+      <c r="N28" s="9">
+        <v>0</v>
+      </c>
+      <c r="O28" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="P28" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="20">
+        <v>0</v>
+      </c>
+      <c r="R28" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="20">
-        <v>0</v>
-      </c>
-      <c r="C28" s="20">
-        <v>0</v>
-      </c>
-      <c r="D28" s="20">
+      <c r="B29" s="20">
+        <v>0</v>
+      </c>
+      <c r="C29" s="20">
+        <v>0</v>
+      </c>
+      <c r="D29" s="20">
         <v>6.5</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E29" s="20">
         <v>1.5</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F29" s="20">
         <v>1</v>
       </c>
-      <c r="H28" s="9">
-        <v>0</v>
-      </c>
-      <c r="I28" s="9">
-        <v>0</v>
-      </c>
-      <c r="J28" s="20">
-        <v>0</v>
-      </c>
-      <c r="K28" s="20">
-        <v>0</v>
-      </c>
-      <c r="L28" s="9">
-        <v>0</v>
-      </c>
-      <c r="N28" s="9">
-        <v>0</v>
-      </c>
-      <c r="O28" s="9">
-        <v>0</v>
-      </c>
-      <c r="P28" s="20">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="20">
-        <v>0</v>
-      </c>
-      <c r="R28" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" s="29" customFormat="1">
-      <c r="B29" s="29">
-        <f>AVERAGE(B18:B28)</f>
+      <c r="H29" s="9">
+        <v>0</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0</v>
+      </c>
+      <c r="J29" s="20">
+        <v>0</v>
+      </c>
+      <c r="K29" s="20">
+        <v>0</v>
+      </c>
+      <c r="L29" s="9">
+        <v>0</v>
+      </c>
+      <c r="N29" s="9">
+        <v>0</v>
+      </c>
+      <c r="O29" s="9">
+        <v>0</v>
+      </c>
+      <c r="P29" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="20">
+        <v>0</v>
+      </c>
+      <c r="R29" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="27" customFormat="1">
+      <c r="B30" s="27">
+        <f>AVERAGE(B19:B29)</f>
         <v>4.8181818181818183</v>
       </c>
-      <c r="C29" s="29">
-        <f>AVERAGE(C18:C28)</f>
+      <c r="C30" s="27">
+        <f>AVERAGE(C19:C29)</f>
         <v>2</v>
       </c>
-      <c r="D29" s="29">
-        <f>AVERAGE(D18:D28)</f>
+      <c r="D30" s="27">
+        <f>AVERAGE(D19:D29)</f>
         <v>2.5454545454545454</v>
       </c>
-      <c r="E29" s="29">
-        <f>AVERAGE(E18:E28)</f>
+      <c r="E30" s="27">
+        <f>AVERAGE(E19:E29)</f>
         <v>2.1363636363636362</v>
       </c>
-      <c r="F29" s="29">
-        <f>AVERAGE(F18:F28)</f>
+      <c r="F30" s="27">
+        <f>AVERAGE(F19:F29)</f>
         <v>1.7272727272727273</v>
       </c>
-      <c r="H29" s="29">
-        <f>AVERAGE(H18:H28)</f>
+      <c r="H30" s="27">
+        <f>AVERAGE(H19:H29)</f>
         <v>1.1818181818181819</v>
       </c>
-      <c r="I29" s="29">
-        <f>AVERAGE(I18:I28)</f>
+      <c r="I30" s="27">
+        <f>AVERAGE(I19:I29)</f>
         <v>0.5</v>
       </c>
-      <c r="J29" s="29">
-        <f>AVERAGE(J18:J28)</f>
+      <c r="J30" s="27">
+        <f>AVERAGE(J19:J29)</f>
         <v>0.95454545454545459</v>
       </c>
-      <c r="K29" s="29">
-        <f>AVERAGE(K18:K28)</f>
+      <c r="K30" s="27">
+        <f>AVERAGE(K19:K29)</f>
         <v>0.72727272727272729</v>
       </c>
-      <c r="L29" s="29">
-        <f>AVERAGE(L18:L28)</f>
+      <c r="L30" s="27">
+        <f>AVERAGE(L19:L29)</f>
         <v>0.31818181818181818</v>
       </c>
-      <c r="N29" s="29">
-        <f>AVERAGE(N18:N28)</f>
+      <c r="N30" s="27">
+        <f>AVERAGE(N19:N29)</f>
         <v>0.77272727272727271</v>
       </c>
-      <c r="O29" s="29">
-        <f>AVERAGE(O18:O28)</f>
+      <c r="O30" s="27">
+        <f>AVERAGE(O19:O29)</f>
         <v>0.68181818181818177</v>
       </c>
-      <c r="P29" s="29">
-        <f>AVERAGE(P18:P28)</f>
+      <c r="P30" s="27">
+        <f>AVERAGE(P19:P29)</f>
         <v>0.45454545454545453</v>
       </c>
-      <c r="Q29" s="29">
-        <f>AVERAGE(Q18:Q28)</f>
+      <c r="Q30" s="27">
+        <f>AVERAGE(Q19:Q29)</f>
         <v>0.5</v>
       </c>
-      <c r="R29" s="29">
-        <f>AVERAGE(R18:R28)</f>
-        <v>0.36363636363636365</v>
+      <c r="R30" s="27">
+        <f>AVERAGE(R19:R29)</f>
+        <v>0.40909090909090912</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="B31" s="29">
+        <f t="shared" ref="B31:R31" si="3" xml:space="preserve"> (B20+B22+B23+B21+B26+B27)/6</f>
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="C31" s="29">
+        <f t="shared" si="3"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="D31" s="29">
+        <f t="shared" si="3"/>
+        <v>3.5833333333333335</v>
+      </c>
+      <c r="E31" s="29">
+        <f t="shared" si="3"/>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="F31" s="29">
+        <f t="shared" si="3"/>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="H31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="J31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="K31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="N31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="O31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="P31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="Q31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="R31" s="29">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -5510,7 +5628,7 @@
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="N2:R2"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Kết quả test với DT ANN mới
</commit_message>
<xml_diff>
--- a/Document/CompResult.xlsx
+++ b/Document/CompResult.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Draft" sheetId="3" r:id="rId3"/>
     <sheet name="Acc" sheetId="5" r:id="rId4"/>
     <sheet name="SERate" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="62">
   <si>
     <t>BT6</t>
   </si>
@@ -638,12 +639,15 @@
   <si>
     <t>2003-2008</t>
   </si>
+  <si>
+    <t>p=5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -796,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -849,6 +853,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,14 +875,25 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -897,9 +913,16 @@
               <a:srgbClr val="C00000"/>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -965,9 +988,16 @@
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1011,41 +1041,59 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="39710080"/>
-        <c:axId val="39711872"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="27306624"/>
+        <c:axId val="27308416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39710080"/>
+        <c:axId val="27306624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39711872"/>
+        <c:crossAx val="27308416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39711872"/>
+        <c:axId val="27308416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39710080"/>
+        <c:crossAx val="27306624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1165,6 +1213,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1199,6 +1248,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1374,21 +1424,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1411,7 +1461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1434,7 +1484,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1457,7 +1507,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1480,7 +1530,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1503,7 +1553,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1524,7 +1574,7 @@
         <v>0.69000000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1541,7 +1591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1558,7 +1608,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1575,7 +1625,7 @@
         <v>0.51500000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1592,7 +1642,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1609,7 +1659,7 @@
         <v>0.48499999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1630,7 +1680,7 @@
         <v>0.5675</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
         <v>42</v>
@@ -1645,7 +1695,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>43</v>
       </c>
@@ -1662,7 +1712,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>44</v>
       </c>
@@ -1687,145 +1737,145 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="26.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="138.5703125" style="6" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="26.25" customHeight="1">
+    <row r="1" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="26.25" customHeight="1">
+    <row r="2" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="26.25" customHeight="1">
+    <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="26.25" customHeight="1">
+    <row r="4" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="26.25" customHeight="1">
+    <row r="5" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="26.25" customHeight="1">
+    <row r="6" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="26.25" customHeight="1">
+    <row r="7" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="26.25" customHeight="1">
+    <row r="8" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="26.25" customHeight="1">
+    <row r="9" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="26.25" customHeight="1">
+    <row r="10" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="26.25" customHeight="1">
+    <row r="11" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="26.25" customHeight="1">
+    <row r="12" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="26.25" customHeight="1">
+    <row r="13" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="26.25" customHeight="1">
+    <row r="14" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="26.25" customHeight="1">
+    <row r="15" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="26.25" customHeight="1">
+    <row r="16" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="26.25" customHeight="1">
+    <row r="17" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="26.25" customHeight="1">
+    <row r="18" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="26.25" customHeight="1">
+    <row r="19" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="26.25" customHeight="1">
+    <row r="20" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="26.25" customHeight="1">
+    <row r="21" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="26.25" customHeight="1">
+    <row r="22" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="26.25" customHeight="1">
+    <row r="23" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="26.25" customHeight="1">
+    <row r="24" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="26.25" customHeight="1">
+    <row r="25" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="26.25" customHeight="1">
+    <row r="26" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
@@ -1840,14 +1890,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="9"/>
     <col min="2" max="2" width="10.85546875" style="9" customWidth="1"/>
@@ -1858,7 +1908,7 @@
     <col min="7" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>58</v>
       </c>
@@ -1882,7 +1932,7 @@
       <c r="Q2" s="31"/>
       <c r="R2" s="31"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1929,7 +1979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>54</v>
       </c>
@@ -1939,7 +1989,7 @@
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>45</v>
       </c>
@@ -1959,7 +2009,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>46</v>
       </c>
@@ -1979,7 +2029,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>0</v>
       </c>
@@ -1999,7 +2049,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
@@ -2019,7 +2069,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>48</v>
       </c>
@@ -2039,7 +2089,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>49</v>
       </c>
@@ -2059,7 +2109,7 @@
         <v>85.5</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>50</v>
       </c>
@@ -2079,7 +2129,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>1</v>
       </c>
@@ -2099,7 +2149,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>51</v>
       </c>
@@ -2119,7 +2169,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>2</v>
       </c>
@@ -2139,7 +2189,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>3</v>
       </c>
@@ -2159,7 +2209,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>52</v>
       </c>
@@ -2179,7 +2229,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>53</v>
       </c>
@@ -2199,7 +2249,7 @@
         <v>90.5</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>56</v>
       </c>
@@ -2219,7 +2269,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
         <f>AVERAGE(B5:B18)</f>
         <v>74.857142857142861</v>
@@ -2281,7 +2331,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>55</v>
       </c>
@@ -2291,7 +2341,7 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>45</v>
       </c>
@@ -2311,7 +2361,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>46</v>
       </c>
@@ -2331,7 +2381,7 @@
         <v>90.5</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -2351,7 +2401,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>47</v>
       </c>
@@ -2371,7 +2421,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>48</v>
       </c>
@@ -2391,7 +2441,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>49</v>
       </c>
@@ -2411,7 +2461,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>50</v>
       </c>
@@ -2431,7 +2481,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>1</v>
       </c>
@@ -2451,7 +2501,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>51</v>
       </c>
@@ -2471,7 +2521,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>2</v>
       </c>
@@ -2491,7 +2541,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>3</v>
       </c>
@@ -2511,7 +2561,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>52</v>
       </c>
@@ -2531,7 +2581,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>53</v>
       </c>
@@ -2551,12 +2601,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B35" s="9">
         <f>AVERAGE(B21:B34)</f>
         <v>56.42307692307692</v>
@@ -2632,14 +2682,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="18"/>
     <col min="2" max="2" width="10.85546875" style="18" customWidth="1"/>
@@ -2653,7 +2703,7 @@
     <col min="14" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>58</v>
       </c>
@@ -2677,7 +2727,7 @@
       <c r="Q2" s="32"/>
       <c r="R2" s="32"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
@@ -2724,7 +2774,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>54</v>
       </c>
@@ -2734,7 +2784,7 @@
       <c r="E4" s="32"/>
       <c r="F4" s="32"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -2787,7 +2837,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="21" customFormat="1">
+    <row r="6" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>0</v>
       </c>
@@ -2840,7 +2890,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="21" customFormat="1">
+    <row r="7" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>47</v>
       </c>
@@ -2893,7 +2943,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="21" customFormat="1">
+    <row r="8" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>48</v>
       </c>
@@ -2946,7 +2996,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="21" customFormat="1">
+    <row r="9" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>49</v>
       </c>
@@ -2999,7 +3049,7 @@
         <v>86.5</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>1</v>
       </c>
@@ -3052,7 +3102,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -3105,7 +3155,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="21" customFormat="1">
+    <row r="12" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>2</v>
       </c>
@@ -3158,7 +3208,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="21" customFormat="1">
+    <row r="13" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>3</v>
       </c>
@@ -3211,7 +3261,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>53</v>
       </c>
@@ -3264,7 +3314,7 @@
         <v>83.5</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>56</v>
       </c>
@@ -3317,7 +3367,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="25" customFormat="1">
+    <row r="16" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="25">
         <f>AVERAGE(B5:B15)</f>
         <v>74.63636363636364</v>
@@ -3379,7 +3429,7 @@
         <v>82.13636363636364</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="28" customFormat="1">
+    <row r="17" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
       <c r="B17" s="29">
         <f t="shared" ref="B17:E17" si="0" xml:space="preserve"> (B6+B8+B9+B7+B12+B13)/6</f>
@@ -3442,7 +3492,7 @@
         <v>82.25</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>45</v>
       </c>
@@ -3495,7 +3545,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>0</v>
       </c>
@@ -3548,7 +3598,7 @@
         <v>78.5</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>47</v>
       </c>
@@ -3601,7 +3651,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>48</v>
       </c>
@@ -3654,7 +3704,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>49</v>
       </c>
@@ -3707,7 +3757,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>1</v>
       </c>
@@ -3760,7 +3810,7 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>51</v>
       </c>
@@ -3813,7 +3863,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>2</v>
       </c>
@@ -3866,7 +3916,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>3</v>
       </c>
@@ -3919,7 +3969,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>53</v>
       </c>
@@ -3972,7 +4022,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>56</v>
       </c>
@@ -4025,7 +4075,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:18" s="25" customFormat="1">
+    <row r="29" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="25">
         <f>AVERAGE(B18:B28)</f>
         <v>57.954545454545453</v>
@@ -4087,7 +4137,7 @@
         <v>76.36363636363636</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="28" customFormat="1">
+    <row r="30" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="29">
         <f t="shared" ref="B30:F30" si="3" xml:space="preserve"> (B19+B21+B22+B20+B25+B26)/6</f>
         <v>54.166666666666664</v>
@@ -4164,14 +4214,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R31"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="20"/>
     <col min="2" max="2" width="10.85546875" style="20" customWidth="1"/>
@@ -4184,7 +4234,7 @@
     <col min="11" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>58</v>
       </c>
@@ -4208,7 +4258,7 @@
       <c r="Q2" s="33"/>
       <c r="R2" s="33"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>9</v>
       </c>
@@ -4255,7 +4305,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>54</v>
       </c>
@@ -4265,7 +4315,7 @@
       <c r="E4" s="33"/>
       <c r="F4" s="33"/>
     </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1">
+    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>45</v>
       </c>
@@ -4316,7 +4366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1">
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>0</v>
       </c>
@@ -4367,7 +4417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>47</v>
       </c>
@@ -4418,7 +4468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1">
+    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>48</v>
       </c>
@@ -4469,7 +4519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1">
+    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>49</v>
       </c>
@@ -4520,7 +4570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1">
+    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>1</v>
       </c>
@@ -4571,7 +4621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1">
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>51</v>
       </c>
@@ -4622,7 +4672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1">
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>2</v>
       </c>
@@ -4673,7 +4723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>3</v>
       </c>
@@ -4724,7 +4774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>53</v>
       </c>
@@ -4775,7 +4825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1">
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>56</v>
       </c>
@@ -4826,7 +4876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="26" customFormat="1">
+    <row r="16" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26">
         <f t="shared" ref="B16:L16" si="0">AVERAGE(B5:B15)</f>
         <v>0.72727272727272729</v>
@@ -4892,7 +4942,7 @@
         <v>0.27272727272727271</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="26" customFormat="1">
+    <row r="17" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="29">
         <f t="shared" ref="B17:L17" si="1" xml:space="preserve"> (B6+B8+B9+B7+B12+B13)/6</f>
         <v>1.25</v>
@@ -4938,7 +4988,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>55</v>
       </c>
@@ -4948,7 +4998,7 @@
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>45</v>
       </c>
@@ -4998,7 +5048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>0</v>
       </c>
@@ -5048,7 +5098,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>47</v>
       </c>
@@ -5098,7 +5148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>48</v>
       </c>
@@ -5148,7 +5198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>49</v>
       </c>
@@ -5198,7 +5248,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>1</v>
       </c>
@@ -5248,7 +5298,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>51</v>
       </c>
@@ -5298,7 +5348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>2</v>
       </c>
@@ -5348,7 +5398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>3</v>
       </c>
@@ -5398,7 +5448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
         <v>53</v>
       </c>
@@ -5448,7 +5498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>56</v>
       </c>
@@ -5498,7 +5548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="27" customFormat="1">
+    <row r="30" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="27">
         <f>AVERAGE(B19:B29)</f>
         <v>4.8181818181818183</v>
@@ -5560,7 +5610,7 @@
         <v>0.40909090909090912</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="29">
         <f t="shared" ref="B31:R31" si="3" xml:space="preserve"> (B20+B22+B23+B21+B26+B27)/6</f>
         <v>8.0833333333333339</v>
@@ -5633,4 +5683,365 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>2003</v>
+      </c>
+      <c r="D1">
+        <v>2004</v>
+      </c>
+      <c r="F1">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>77.25</v>
+      </c>
+      <c r="D2">
+        <v>66.5</v>
+      </c>
+      <c r="F2">
+        <v>62.68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>69.23</v>
+      </c>
+      <c r="D3">
+        <v>74</v>
+      </c>
+      <c r="F3">
+        <v>67.91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>78.59</v>
+      </c>
+      <c r="D4">
+        <v>62</v>
+      </c>
+      <c r="F4" s="34">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>77.59</v>
+      </c>
+      <c r="D5">
+        <v>79.5</v>
+      </c>
+      <c r="F5">
+        <v>72.39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>78.92</v>
+      </c>
+      <c r="D6">
+        <v>88.5</v>
+      </c>
+      <c r="F6">
+        <v>85.07</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>84.94</v>
+      </c>
+      <c r="D7">
+        <v>62</v>
+      </c>
+      <c r="F7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>88.96</v>
+      </c>
+      <c r="D8">
+        <v>90.5</v>
+      </c>
+      <c r="F8">
+        <v>85.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>67.22</v>
+      </c>
+      <c r="D9">
+        <v>76.5</v>
+      </c>
+      <c r="F9">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>76.58</v>
+      </c>
+      <c r="D10">
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <v>69.400000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11">
+        <v>79.260000000000005</v>
+      </c>
+      <c r="D11">
+        <v>85.5</v>
+      </c>
+      <c r="F11">
+        <v>78.349999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="D12">
+        <v>88.5</v>
+      </c>
+      <c r="F12">
+        <v>88.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>78.194545454545462</v>
+      </c>
+      <c r="D13">
+        <v>77.13636363636364</v>
+      </c>
+      <c r="F13">
+        <v>72.470909090909103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>68</v>
+      </c>
+      <c r="F15">
+        <v>82.09</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>61</v>
+      </c>
+      <c r="D16">
+        <v>60.5</v>
+      </c>
+      <c r="F16">
+        <v>62.68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>58</v>
+      </c>
+      <c r="D17">
+        <v>23</v>
+      </c>
+      <c r="F17">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18">
+        <v>79.5</v>
+      </c>
+      <c r="D18">
+        <v>73</v>
+      </c>
+      <c r="F18">
+        <v>71.64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>74.5</v>
+      </c>
+      <c r="D19">
+        <v>76</v>
+      </c>
+      <c r="F19">
+        <v>70.150000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>70.5</v>
+      </c>
+      <c r="D20">
+        <v>58.5</v>
+      </c>
+      <c r="F20">
+        <v>33.58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>92</v>
+      </c>
+      <c r="D21">
+        <v>89</v>
+      </c>
+      <c r="F21">
+        <v>49.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>73</v>
+      </c>
+      <c r="D22">
+        <v>61</v>
+      </c>
+      <c r="F22">
+        <v>60.45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>80.5</v>
+      </c>
+      <c r="D23">
+        <v>69</v>
+      </c>
+      <c r="F23">
+        <v>24.62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24">
+        <v>86.5</v>
+      </c>
+      <c r="D24">
+        <v>79.5</v>
+      </c>
+      <c r="F24">
+        <v>70.150000000000006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <v>79</v>
+      </c>
+      <c r="D25">
+        <v>78.5</v>
+      </c>
+      <c r="F25">
+        <v>72.38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>74.954545454545453</v>
+      </c>
+      <c r="D26">
+        <v>66.909090909090907</v>
+      </c>
+      <c r="F26">
+        <v>55.017272727272719</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật lại kết quả test với code DT ANN mới
</commit_message>
<xml_diff>
--- a/Document/CompResult.xlsx
+++ b/Document/CompResult.xlsx
@@ -844,6 +844,7 @@
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -853,7 +854,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,11 +1050,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="27306624"/>
-        <c:axId val="27308416"/>
+        <c:axId val="67326336"/>
+        <c:axId val="67328640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="27306624"/>
+        <c:axId val="67326336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1063,7 +1063,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="27308416"/>
+        <c:crossAx val="67328640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1071,7 +1071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27308416"/>
+        <c:axId val="67328640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1082,7 +1082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="27306624"/>
+        <c:crossAx val="67326336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1909,28 +1909,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="H2" s="31" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="H2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="N2" s="31" t="s">
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="N2" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -1980,14 +1980,14 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -2332,14 +2332,14 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
@@ -2685,8 +2685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="D7" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2704,28 +2704,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="H2" s="32" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="N2" s="32" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
@@ -2775,14 +2775,14 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -4235,28 +4235,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="H2" s="33" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="H2" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="N2" s="33" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="N2" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
@@ -4306,14 +4306,14 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
@@ -4989,14 +4989,14 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
@@ -5687,15 +5687,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>2003</v>
       </c>
@@ -5706,247 +5709,255 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>45</v>
       </c>
       <c r="B2">
-        <v>77.25</v>
+        <v>83.5</v>
       </c>
       <c r="D2">
-        <v>66.5</v>
+        <v>78.5</v>
       </c>
       <c r="F2">
-        <v>62.68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>69.23</v>
+        <v>74</v>
       </c>
       <c r="D3">
-        <v>74</v>
+        <v>74.5</v>
       </c>
       <c r="F3">
-        <v>67.91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B4">
-        <v>78.59</v>
+        <v>85</v>
       </c>
       <c r="D4">
-        <v>62</v>
-      </c>
-      <c r="F4" s="34">
-        <v>52.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64.5</v>
+      </c>
+      <c r="F4" s="31">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>48</v>
       </c>
       <c r="B5">
-        <v>77.59</v>
+        <v>83.5</v>
       </c>
       <c r="D5">
-        <v>79.5</v>
+        <v>84.5</v>
       </c>
       <c r="F5">
-        <v>72.39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B6">
-        <v>78.92</v>
+        <v>92</v>
       </c>
       <c r="D6">
-        <v>88.5</v>
+        <v>89</v>
       </c>
       <c r="F6">
-        <v>85.07</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>84.94</v>
+        <v>82</v>
       </c>
       <c r="D7">
-        <v>62</v>
+        <v>66.5</v>
       </c>
       <c r="F7">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B8">
-        <v>88.96</v>
+        <v>95</v>
       </c>
       <c r="D8">
-        <v>90.5</v>
+        <v>95</v>
       </c>
       <c r="F8">
-        <v>85.82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B9">
-        <v>67.22</v>
+        <v>83</v>
       </c>
       <c r="D9">
-        <v>76.5</v>
+        <v>87</v>
       </c>
       <c r="F9">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B10">
-        <v>76.58</v>
+        <v>83</v>
       </c>
       <c r="D10">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="F10">
-        <v>69.400000000000006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>53</v>
       </c>
       <c r="B11">
-        <v>79.260000000000005</v>
+        <v>88</v>
       </c>
       <c r="D11">
+        <v>87.5</v>
+      </c>
+      <c r="F11">
         <v>85.5</v>
       </c>
-      <c r="F11">
-        <v>78.349999999999994</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B12">
-        <v>81.599999999999994</v>
+        <v>91</v>
       </c>
       <c r="D12">
-        <v>88.5</v>
+        <v>92</v>
       </c>
       <c r="F12">
-        <v>88.06</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>78.194545454545462</v>
+        <f t="shared" ref="B13" si="0">AVERAGE(B2:B12)</f>
+        <v>85.454545454545453</v>
       </c>
       <c r="D13">
-        <v>77.13636363636364</v>
+        <f t="shared" ref="D13:E13" si="1">AVERAGE(D2:D12)</f>
+        <v>82.36363636363636</v>
       </c>
       <c r="F13">
-        <v>72.470909090909103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <f>AVERAGE(F2:F12)</f>
+        <v>80.590909090909093</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>45</v>
       </c>
       <c r="B15">
-        <v>70</v>
+        <v>82.5</v>
       </c>
       <c r="D15">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="F15">
-        <v>82.09</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82.5</v>
+      </c>
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B16">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D16">
-        <v>60.5</v>
+        <v>62.5</v>
       </c>
       <c r="F16">
-        <v>62.68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B17">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="D17">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="F17">
-        <v>8.1999999999999993</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>48</v>
       </c>
       <c r="B18">
-        <v>79.5</v>
+        <v>83</v>
       </c>
       <c r="D18">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F18">
-        <v>71.64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B19">
-        <v>74.5</v>
+        <v>84</v>
       </c>
       <c r="D19">
-        <v>76</v>
+        <v>78.5</v>
       </c>
       <c r="F19">
-        <v>70.150000000000006</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>78.5</v>
+      </c>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>1</v>
       </c>
@@ -5954,55 +5965,59 @@
         <v>70.5</v>
       </c>
       <c r="D20">
-        <v>58.5</v>
+        <v>54.5</v>
       </c>
       <c r="F20">
-        <v>33.58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B21">
+        <v>90</v>
+      </c>
+      <c r="D21">
+        <v>91.5</v>
+      </c>
+      <c r="F21">
         <v>92</v>
       </c>
-      <c r="D21">
-        <v>89</v>
-      </c>
-      <c r="F21">
-        <v>49.25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B22">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D22">
-        <v>61</v>
+        <v>81.5</v>
       </c>
       <c r="F22">
-        <v>60.45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70.5</v>
+      </c>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B23">
-        <v>80.5</v>
+        <v>82</v>
       </c>
       <c r="D23">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F23">
-        <v>24.62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>53</v>
       </c>
@@ -6010,36 +6025,42 @@
         <v>86.5</v>
       </c>
       <c r="D24">
-        <v>79.5</v>
+        <v>81.5</v>
       </c>
       <c r="F24">
-        <v>70.150000000000006</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B25">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D25">
-        <v>78.5</v>
+        <v>83.5</v>
       </c>
       <c r="F25">
-        <v>72.38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>74.954545454545453</v>
+        <f t="shared" ref="B26:E26" si="2">AVERAGE(B15:B25)</f>
+        <v>80.772727272727266</v>
       </c>
       <c r="D26">
-        <v>66.909090909090907</v>
+        <f t="shared" si="2"/>
+        <v>77.045454545454547</v>
       </c>
       <c r="F26">
-        <v>55.017272727272719</v>
-      </c>
+        <f>AVERAGE(F15:F25)</f>
+        <v>74.5</v>
+      </c>
+      <c r="G26" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cập nhật SERate DT-ANN
</commit_message>
<xml_diff>
--- a/Document/CompResult.xlsx
+++ b/Document/CompResult.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Draft" sheetId="3" r:id="rId3"/>
     <sheet name="Acc" sheetId="5" r:id="rId4"/>
     <sheet name="SERate" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
+    <sheet name="DT-ANN" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="63">
   <si>
     <t>BT6</t>
   </si>
@@ -642,6 +642,9 @@
   <si>
     <t>p=5</t>
   </si>
+  <si>
+    <t>SERate</t>
+  </si>
 </sst>
 </file>
 
@@ -1050,11 +1053,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="67326336"/>
-        <c:axId val="67328640"/>
+        <c:axId val="71511040"/>
+        <c:axId val="71525120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67326336"/>
+        <c:axId val="71511040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1063,7 +1066,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67328640"/>
+        <c:crossAx val="71525120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1071,7 +1074,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67328640"/>
+        <c:axId val="71525120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1082,7 +1085,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67326336"/>
+        <c:crossAx val="71511040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2685,7 +2688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
@@ -4217,7 +4220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R31"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
@@ -5687,10 +5690,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5698,369 +5701,591 @@
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>2003</v>
       </c>
+      <c r="C1">
+        <v>2004</v>
+      </c>
       <c r="D1">
+        <v>2005</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1">
+        <v>2003</v>
+      </c>
+      <c r="G1">
         <v>2004</v>
       </c>
-      <c r="F1">
+      <c r="H1">
         <v>2005</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>45</v>
       </c>
       <c r="B2">
         <v>83.5</v>
       </c>
+      <c r="C2">
+        <v>78.5</v>
+      </c>
       <c r="D2">
-        <v>78.5</v>
+        <v>80</v>
       </c>
       <c r="F2">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <v>74</v>
       </c>
+      <c r="C3">
+        <v>74.5</v>
+      </c>
       <c r="D3">
-        <v>74.5</v>
+        <v>72</v>
       </c>
       <c r="F3">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B4">
         <v>85</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>64.5</v>
       </c>
-      <c r="F4" s="31">
+      <c r="D4" s="31">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>3.5</v>
+      </c>
+      <c r="H4">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>48</v>
       </c>
       <c r="B5">
         <v>83.5</v>
       </c>
+      <c r="C5">
+        <v>84.5</v>
+      </c>
       <c r="D5">
-        <v>84.5</v>
+        <v>85.5</v>
       </c>
       <c r="F5">
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B6">
         <v>92</v>
       </c>
+      <c r="C6">
+        <v>89</v>
+      </c>
       <c r="D6">
         <v>89</v>
       </c>
       <c r="F6">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B7">
         <v>82</v>
       </c>
+      <c r="C7">
+        <v>66.5</v>
+      </c>
       <c r="D7">
-        <v>66.5</v>
+        <v>63</v>
       </c>
       <c r="F7">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B8">
         <v>95</v>
       </c>
+      <c r="C8">
+        <v>95</v>
+      </c>
       <c r="D8">
-        <v>95</v>
+        <v>93.5</v>
       </c>
       <c r="F8">
-        <v>93.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B9">
         <v>83</v>
       </c>
+      <c r="C9">
+        <v>87</v>
+      </c>
       <c r="D9">
-        <v>87</v>
+        <v>81.5</v>
       </c>
       <c r="F9">
-        <v>81.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B10">
         <v>83</v>
       </c>
+      <c r="C10">
+        <v>87</v>
+      </c>
       <c r="D10">
-        <v>87</v>
+        <v>84.5</v>
       </c>
       <c r="F10">
-        <v>84.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>53</v>
       </c>
       <c r="B11">
         <v>88</v>
       </c>
+      <c r="C11">
+        <v>87.5</v>
+      </c>
       <c r="D11">
-        <v>87.5</v>
+        <v>85.5</v>
       </c>
       <c r="F11">
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B12">
         <v>91</v>
       </c>
+      <c r="C12">
+        <v>92</v>
+      </c>
       <c r="D12">
         <v>92</v>
       </c>
       <c r="F12">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" ref="B13" si="0">AVERAGE(B2:B12)</f>
         <v>85.454545454545453</v>
       </c>
+      <c r="C13">
+        <f t="shared" ref="C13" si="1">AVERAGE(C2:C12)</f>
+        <v>82.36363636363636</v>
+      </c>
       <c r="D13">
-        <f t="shared" ref="D13:E13" si="1">AVERAGE(D2:D12)</f>
-        <v>82.36363636363636</v>
+        <f>AVERAGE(D2:D12)</f>
+        <v>80.590909090909093</v>
       </c>
       <c r="F13">
-        <f>AVERAGE(F2:F12)</f>
-        <v>80.590909090909093</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E13:H13" si="2">AVERAGE(F2:F12)</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>45</v>
       </c>
       <c r="B15">
         <v>82.5</v>
       </c>
+      <c r="C15">
+        <v>80</v>
+      </c>
       <c r="D15">
-        <v>80</v>
+        <v>82.5</v>
       </c>
       <c r="F15">
-        <v>82.5</v>
-      </c>
-      <c r="G15" s="19"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G15" s="19">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B16">
         <v>64</v>
       </c>
+      <c r="C16">
+        <v>62.5</v>
+      </c>
       <c r="D16">
-        <v>62.5</v>
+        <v>64</v>
       </c>
       <c r="F16">
-        <v>64</v>
-      </c>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B17">
         <v>80</v>
       </c>
+      <c r="C17">
+        <v>80</v>
+      </c>
       <c r="D17">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F17">
-        <v>60</v>
-      </c>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>48</v>
       </c>
       <c r="B18">
         <v>83</v>
       </c>
+      <c r="C18">
+        <v>81</v>
+      </c>
       <c r="D18">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F18">
-        <v>84</v>
-      </c>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B19">
         <v>84</v>
       </c>
+      <c r="C19">
+        <v>78.5</v>
+      </c>
       <c r="D19">
         <v>78.5</v>
       </c>
       <c r="F19">
-        <v>78.5</v>
-      </c>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G19" s="18">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B20">
         <v>70.5</v>
       </c>
+      <c r="C20">
+        <v>54.5</v>
+      </c>
       <c r="D20">
-        <v>54.5</v>
+        <v>54</v>
       </c>
       <c r="F20">
-        <v>54</v>
-      </c>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G20" s="18">
+        <v>6.5</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B21">
         <v>90</v>
       </c>
+      <c r="C21">
+        <v>91.5</v>
+      </c>
       <c r="D21">
-        <v>91.5</v>
+        <v>92</v>
       </c>
       <c r="F21">
-        <v>92</v>
-      </c>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B22">
         <v>82</v>
       </c>
+      <c r="C22">
+        <v>81.5</v>
+      </c>
       <c r="D22">
-        <v>81.5</v>
+        <v>70.5</v>
       </c>
       <c r="F22">
-        <v>70.5</v>
-      </c>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B23">
         <v>82</v>
       </c>
+      <c r="C23">
+        <v>73</v>
+      </c>
       <c r="D23">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F23">
-        <v>67</v>
-      </c>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G23" s="18">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>53</v>
       </c>
       <c r="B24">
         <v>86.5</v>
       </c>
+      <c r="C24">
+        <v>81.5</v>
+      </c>
       <c r="D24">
-        <v>81.5</v>
+        <v>82</v>
       </c>
       <c r="F24">
-        <v>82</v>
-      </c>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G24" s="18">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B25">
         <v>84</v>
       </c>
+      <c r="C25">
+        <v>83.5</v>
+      </c>
       <c r="D25">
-        <v>83.5</v>
+        <v>85</v>
       </c>
       <c r="F25">
-        <v>85</v>
-      </c>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G25" s="18">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26">
-        <f t="shared" ref="B26:E26" si="2">AVERAGE(B15:B25)</f>
+        <f t="shared" ref="B26:D26" si="3">AVERAGE(B15:B25)</f>
         <v>80.772727272727266</v>
       </c>
+      <c r="C26">
+        <f>AVERAGE(C15:C25)</f>
+        <v>77.045454545454547</v>
+      </c>
       <c r="D26">
-        <f t="shared" si="2"/>
-        <v>77.045454545454547</v>
+        <f>AVERAGE(D15:D25)</f>
+        <v>74.5</v>
       </c>
       <c r="F26">
-        <f>AVERAGE(F15:F25)</f>
-        <v>74.5</v>
-      </c>
-      <c r="G26" s="25"/>
+        <f t="shared" ref="E26:H26" si="4">AVERAGE(F15:F25)</f>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>2.6818181818181817</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Câp nhật kết quả test dt-ann mới
</commit_message>
<xml_diff>
--- a/Document/CompResult.xlsx
+++ b/Document/CompResult.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" activeTab="5"/>
@@ -14,12 +14,12 @@
     <sheet name="SERate" sheetId="4" r:id="rId5"/>
     <sheet name="DT-ANN" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="62">
   <si>
     <t>BT6</t>
   </si>
@@ -640,17 +640,14 @@
     <t>2003-2008</t>
   </si>
   <si>
-    <t>p=5</t>
-  </si>
-  <si>
     <t>SERate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,8 +739,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -762,8 +766,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -799,11 +809,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -847,7 +909,6 @@
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -857,6 +918,19 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,25 +952,14 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="18"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -916,16 +979,9 @@
               <a:srgbClr val="C00000"/>
             </a:solidFill>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -991,16 +1047,9 @@
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1044,63 +1093,45 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="71511040"/>
-        <c:axId val="71525120"/>
+        <c:axId val="44940672"/>
+        <c:axId val="45028480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71511040"/>
+        <c:axId val="44940672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71525120"/>
+        <c:crossAx val="45028480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71525120"/>
+        <c:axId val="45028480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71511040"/>
+        <c:crossAx val="44940672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1216,7 +1247,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1251,7 +1281,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1427,21 +1456,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1464,7 +1493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1487,7 +1516,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1510,7 +1539,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1533,7 +1562,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1556,7 +1585,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1577,7 +1606,7 @@
         <v>0.69000000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1594,7 +1623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1611,7 +1640,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1628,7 +1657,7 @@
         <v>0.51500000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1645,7 +1674,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1662,7 +1691,7 @@
         <v>0.48499999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1683,7 +1712,7 @@
         <v>0.5675</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
         <v>42</v>
@@ -1698,7 +1727,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="9" t="s">
         <v>43</v>
       </c>
@@ -1715,7 +1744,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="9" t="s">
         <v>44</v>
       </c>
@@ -1740,145 +1769,145 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="26.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="138.5703125" style="6" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="26.25" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="26.25" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="26.25" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="26.25" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="26.25" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="26.25" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="26.25" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="26.25" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="26.25" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="26.25" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="26.25" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="26.25" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="26.25" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="26.25" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="26.25" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="26.25" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="26.25" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="26.25" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="26.25" customHeight="1">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="26.25" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="26.25" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="26.25" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="26.25" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="26.25" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="26.25" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="26.25" customHeight="1">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
@@ -1893,14 +1922,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R35"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="9"/>
     <col min="2" max="2" width="10.85546875" style="9" customWidth="1"/>
@@ -1911,31 +1940,31 @@
     <col min="7" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:18">
+      <c r="A2" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="H2" s="32" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="H2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="N2" s="32" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="N2" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1982,17 +2011,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:18">
+      <c r="A4" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="9" t="s">
         <v>45</v>
       </c>
@@ -2012,7 +2041,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6" s="9" t="s">
         <v>46</v>
       </c>
@@ -2032,7 +2061,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7" s="10" t="s">
         <v>0</v>
       </c>
@@ -2052,7 +2081,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
@@ -2072,7 +2101,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9" s="9" t="s">
         <v>48</v>
       </c>
@@ -2092,7 +2121,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" s="9" t="s">
         <v>49</v>
       </c>
@@ -2112,7 +2141,7 @@
         <v>85.5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" s="9" t="s">
         <v>50</v>
       </c>
@@ -2132,7 +2161,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12" s="10" t="s">
         <v>1</v>
       </c>
@@ -2152,7 +2181,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13" s="9" t="s">
         <v>51</v>
       </c>
@@ -2172,7 +2201,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="A14" s="10" t="s">
         <v>2</v>
       </c>
@@ -2192,7 +2221,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15" s="10" t="s">
         <v>3</v>
       </c>
@@ -2212,7 +2241,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="A16" s="9" t="s">
         <v>52</v>
       </c>
@@ -2232,7 +2261,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18">
       <c r="A17" s="9" t="s">
         <v>53</v>
       </c>
@@ -2252,7 +2281,7 @@
         <v>90.5</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18">
       <c r="A18" s="9" t="s">
         <v>56</v>
       </c>
@@ -2272,7 +2301,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18">
       <c r="B19" s="9">
         <f>AVERAGE(B5:B18)</f>
         <v>74.857142857142861</v>
@@ -2334,17 +2363,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+    <row r="20" spans="1:18">
+      <c r="A20" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="9" t="s">
         <v>45</v>
       </c>
@@ -2364,7 +2393,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18">
       <c r="A22" s="9" t="s">
         <v>46</v>
       </c>
@@ -2384,7 +2413,7 @@
         <v>90.5</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -2404,7 +2433,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18">
       <c r="A24" s="9" t="s">
         <v>47</v>
       </c>
@@ -2424,7 +2453,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18">
       <c r="A25" s="9" t="s">
         <v>48</v>
       </c>
@@ -2444,7 +2473,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18">
       <c r="A26" s="9" t="s">
         <v>49</v>
       </c>
@@ -2464,7 +2493,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18">
       <c r="A27" s="9" t="s">
         <v>50</v>
       </c>
@@ -2484,7 +2513,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18">
       <c r="A28" s="10" t="s">
         <v>1</v>
       </c>
@@ -2504,7 +2533,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18">
       <c r="A29" s="9" t="s">
         <v>51</v>
       </c>
@@ -2524,7 +2553,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18">
       <c r="A30" s="10" t="s">
         <v>2</v>
       </c>
@@ -2544,7 +2573,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18">
       <c r="A31" s="10" t="s">
         <v>3</v>
       </c>
@@ -2564,7 +2593,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18">
       <c r="A32" s="9" t="s">
         <v>52</v>
       </c>
@@ -2584,7 +2613,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18">
       <c r="A33" s="9" t="s">
         <v>53</v>
       </c>
@@ -2604,12 +2633,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18">
       <c r="A34" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18">
       <c r="B35" s="9">
         <f>AVERAGE(B21:B34)</f>
         <v>56.42307692307692</v>
@@ -2685,14 +2714,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R30"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="18"/>
     <col min="2" max="2" width="10.85546875" style="18" customWidth="1"/>
@@ -2706,31 +2735,31 @@
     <col min="14" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+    <row r="2" spans="1:18">
+      <c r="A2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="H2" s="33" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="H2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="N2" s="33" t="s">
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="N2" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
@@ -2777,17 +2806,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:18">
+      <c r="A4" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="18" t="s">
         <v>45</v>
       </c>
@@ -2840,7 +2869,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="21" customFormat="1">
       <c r="A6" s="21" t="s">
         <v>0</v>
       </c>
@@ -2893,7 +2922,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="21" customFormat="1">
       <c r="A7" s="21" t="s">
         <v>47</v>
       </c>
@@ -2946,7 +2975,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="21" customFormat="1">
       <c r="A8" s="21" t="s">
         <v>48</v>
       </c>
@@ -2999,7 +3028,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="21" customFormat="1">
       <c r="A9" s="21" t="s">
         <v>49</v>
       </c>
@@ -3052,7 +3081,7 @@
         <v>86.5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" s="18" t="s">
         <v>1</v>
       </c>
@@ -3105,7 +3134,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
@@ -3158,7 +3187,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="21" customFormat="1">
       <c r="A12" s="21" t="s">
         <v>2</v>
       </c>
@@ -3211,7 +3240,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="21" customFormat="1">
       <c r="A13" s="21" t="s">
         <v>3</v>
       </c>
@@ -3264,7 +3293,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="A14" s="18" t="s">
         <v>53</v>
       </c>
@@ -3317,7 +3346,7 @@
         <v>83.5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15" s="18" t="s">
         <v>56</v>
       </c>
@@ -3370,7 +3399,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="25" customFormat="1">
       <c r="B16" s="25">
         <f>AVERAGE(B5:B15)</f>
         <v>74.63636363636364</v>
@@ -3432,7 +3461,7 @@
         <v>82.13636363636364</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="28" customFormat="1">
       <c r="A17" s="30"/>
       <c r="B17" s="29">
         <f t="shared" ref="B17:E17" si="0" xml:space="preserve"> (B6+B8+B9+B7+B12+B13)/6</f>
@@ -3495,7 +3524,7 @@
         <v>82.25</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18">
       <c r="A18" s="18" t="s">
         <v>45</v>
       </c>
@@ -3548,7 +3577,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18">
       <c r="A19" s="18" t="s">
         <v>0</v>
       </c>
@@ -3601,7 +3630,7 @@
         <v>78.5</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18">
       <c r="A20" s="18" t="s">
         <v>47</v>
       </c>
@@ -3654,7 +3683,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18">
       <c r="A21" s="18" t="s">
         <v>48</v>
       </c>
@@ -3707,7 +3736,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18">
       <c r="A22" s="18" t="s">
         <v>49</v>
       </c>
@@ -3760,7 +3789,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18">
       <c r="A23" s="18" t="s">
         <v>1</v>
       </c>
@@ -3813,7 +3842,7 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18">
       <c r="A24" s="18" t="s">
         <v>51</v>
       </c>
@@ -3866,7 +3895,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18">
       <c r="A25" s="18" t="s">
         <v>2</v>
       </c>
@@ -3919,7 +3948,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18">
       <c r="A26" s="18" t="s">
         <v>3</v>
       </c>
@@ -3972,7 +4001,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18">
       <c r="A27" s="18" t="s">
         <v>53</v>
       </c>
@@ -4025,7 +4054,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18">
       <c r="A28" s="18" t="s">
         <v>56</v>
       </c>
@@ -4078,7 +4107,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" s="25" customFormat="1">
       <c r="B29" s="25">
         <f>AVERAGE(B18:B28)</f>
         <v>57.954545454545453</v>
@@ -4140,7 +4169,7 @@
         <v>76.36363636363636</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" s="28" customFormat="1">
       <c r="B30" s="29">
         <f t="shared" ref="B30:F30" si="3" xml:space="preserve"> (B19+B21+B22+B20+B25+B26)/6</f>
         <v>54.166666666666664</v>
@@ -4217,14 +4246,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="20"/>
     <col min="2" max="2" width="10.85546875" style="20" customWidth="1"/>
@@ -4237,31 +4266,31 @@
     <col min="11" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:18">
+      <c r="A2" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="H2" s="34" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="N2" s="34" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="B3" s="20" t="s">
         <v>9</v>
       </c>
@@ -4308,17 +4337,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A4" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" thickBot="1">
       <c r="A5" s="20" t="s">
         <v>45</v>
       </c>
@@ -4369,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="15.75" thickBot="1">
       <c r="A6" s="20" t="s">
         <v>0</v>
       </c>
@@ -4420,7 +4449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1">
       <c r="A7" s="20" t="s">
         <v>47</v>
       </c>
@@ -4471,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="15.75" thickBot="1">
       <c r="A8" s="20" t="s">
         <v>48</v>
       </c>
@@ -4522,7 +4551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="15.75" thickBot="1">
       <c r="A9" s="20" t="s">
         <v>49</v>
       </c>
@@ -4573,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="15.75" thickBot="1">
       <c r="A10" s="20" t="s">
         <v>1</v>
       </c>
@@ -4624,7 +4653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="15.75" thickBot="1">
       <c r="A11" s="20" t="s">
         <v>51</v>
       </c>
@@ -4675,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="15.75" thickBot="1">
       <c r="A12" s="20" t="s">
         <v>2</v>
       </c>
@@ -4726,7 +4755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1">
       <c r="A13" s="20" t="s">
         <v>3</v>
       </c>
@@ -4777,7 +4806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1">
       <c r="A14" s="20" t="s">
         <v>53</v>
       </c>
@@ -4828,7 +4857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="15.75" thickBot="1">
       <c r="A15" s="20" t="s">
         <v>56</v>
       </c>
@@ -4879,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="26" customFormat="1">
       <c r="B16" s="26">
         <f t="shared" ref="B16:L16" si="0">AVERAGE(B5:B15)</f>
         <v>0.72727272727272729</v>
@@ -4945,7 +4974,7 @@
         <v>0.27272727272727271</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="26" customFormat="1">
       <c r="B17" s="29">
         <f t="shared" ref="B17:L17" si="1" xml:space="preserve"> (B6+B8+B9+B7+B12+B13)/6</f>
         <v>1.25</v>
@@ -4991,17 +5020,17 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+    <row r="18" spans="1:18">
+      <c r="A18" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="20" t="s">
         <v>45</v>
       </c>
@@ -5051,7 +5080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18">
       <c r="A20" s="20" t="s">
         <v>0</v>
       </c>
@@ -5101,7 +5130,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18">
       <c r="A21" s="20" t="s">
         <v>47</v>
       </c>
@@ -5151,7 +5180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18">
       <c r="A22" s="20" t="s">
         <v>48</v>
       </c>
@@ -5201,7 +5230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18">
       <c r="A23" s="20" t="s">
         <v>49</v>
       </c>
@@ -5251,7 +5280,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18">
       <c r="A24" s="20" t="s">
         <v>1</v>
       </c>
@@ -5301,7 +5330,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18">
       <c r="A25" s="20" t="s">
         <v>51</v>
       </c>
@@ -5351,7 +5380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18">
       <c r="A26" s="20" t="s">
         <v>2</v>
       </c>
@@ -5401,7 +5430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18">
       <c r="A27" s="20" t="s">
         <v>3</v>
       </c>
@@ -5451,7 +5480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18">
       <c r="A28" s="20" t="s">
         <v>53</v>
       </c>
@@ -5501,7 +5530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18">
       <c r="A29" s="20" t="s">
         <v>56</v>
       </c>
@@ -5551,7 +5580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" s="27" customFormat="1">
       <c r="B30" s="27">
         <f>AVERAGE(B19:B29)</f>
         <v>4.8181818181818183</v>
@@ -5613,7 +5642,7 @@
         <v>0.40909090909090912</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18">
       <c r="B31" s="29">
         <f t="shared" ref="B31:R31" si="3" xml:space="preserve"> (B20+B22+B23+B21+B26+B27)/6</f>
         <v>8.0833333333333339</v>
@@ -5689,605 +5718,638 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1">
+    <row r="1" spans="1:8">
+      <c r="A1" s="34"/>
+      <c r="B1" s="35">
+        <v>2005</v>
+      </c>
+      <c r="C1" s="36">
+        <v>2004</v>
+      </c>
+      <c r="D1" s="35">
         <v>2003</v>
       </c>
-      <c r="C1">
+      <c r="E1" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="35">
+        <v>2005</v>
+      </c>
+      <c r="G1" s="36">
         <v>2004</v>
       </c>
-      <c r="D1">
-        <v>2005</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1">
+      <c r="H1" s="35">
         <v>2003</v>
       </c>
-      <c r="G1">
-        <v>2004</v>
-      </c>
-      <c r="H1">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B2">
-        <v>83.5</v>
-      </c>
-      <c r="C2">
-        <v>78.5</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="39">
+        <v>77.5</v>
+      </c>
+      <c r="C2" s="40">
+        <v>63</v>
+      </c>
+      <c r="D2" s="41">
         <v>80</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>74</v>
-      </c>
-      <c r="C3">
+      <c r="E2" s="40"/>
+      <c r="F2" s="41">
+        <v>0</v>
+      </c>
+      <c r="G2" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="41">
+        <v>69</v>
+      </c>
+      <c r="C3" s="40">
+        <v>71</v>
+      </c>
+      <c r="D3" s="41">
+        <v>72</v>
+      </c>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41">
+        <v>0</v>
+      </c>
+      <c r="G3" s="40">
+        <v>0</v>
+      </c>
+      <c r="H3" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="39">
+        <v>41</v>
+      </c>
+      <c r="C4" s="43">
+        <v>57</v>
+      </c>
+      <c r="D4" s="41">
+        <v>76.5</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="44">
+        <v>19.5</v>
+      </c>
+      <c r="G4" s="40">
+        <v>4</v>
+      </c>
+      <c r="H4" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="39">
+        <v>82.5</v>
+      </c>
+      <c r="C5" s="40">
+        <v>84.5</v>
+      </c>
+      <c r="D5" s="41">
+        <v>84</v>
+      </c>
+      <c r="E5" s="40"/>
+      <c r="F5" s="41">
+        <v>0</v>
+      </c>
+      <c r="G5" s="40">
+        <v>0</v>
+      </c>
+      <c r="H5" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="39">
+        <v>87</v>
+      </c>
+      <c r="C6" s="40">
+        <v>75.5</v>
+      </c>
+      <c r="D6" s="41">
+        <v>89</v>
+      </c>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41">
+        <v>0</v>
+      </c>
+      <c r="G6" s="40">
+        <v>0</v>
+      </c>
+      <c r="H6" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="41">
+        <v>57.5</v>
+      </c>
+      <c r="C7" s="40">
+        <v>63</v>
+      </c>
+      <c r="D7" s="41">
+        <v>73</v>
+      </c>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41">
+        <v>0</v>
+      </c>
+      <c r="G7" s="40">
+        <v>0</v>
+      </c>
+      <c r="H7" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="39">
+        <v>89.5</v>
+      </c>
+      <c r="C8" s="45">
+        <v>91.5</v>
+      </c>
+      <c r="D8" s="41">
+        <v>93</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41">
+        <v>0</v>
+      </c>
+      <c r="G8" s="40">
+        <v>0</v>
+      </c>
+      <c r="H8" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="39">
+        <v>79.5</v>
+      </c>
+      <c r="C9" s="40">
+        <v>80</v>
+      </c>
+      <c r="D9" s="41">
+        <v>79</v>
+      </c>
+      <c r="E9" s="40"/>
+      <c r="F9" s="41">
+        <v>0</v>
+      </c>
+      <c r="G9" s="40">
+        <v>0</v>
+      </c>
+      <c r="H9" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="39">
+        <v>78</v>
+      </c>
+      <c r="C10" s="40">
+        <v>76</v>
+      </c>
+      <c r="D10" s="41">
+        <v>83</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41">
+        <v>2.5</v>
+      </c>
+      <c r="G10" s="40">
+        <v>1</v>
+      </c>
+      <c r="H10" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="39">
+        <v>81.5</v>
+      </c>
+      <c r="C11" s="40">
+        <v>87.5</v>
+      </c>
+      <c r="D11" s="41">
+        <v>85.5</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="41">
+        <v>0</v>
+      </c>
+      <c r="G11" s="40">
+        <v>0</v>
+      </c>
+      <c r="H11" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="39">
+        <v>90</v>
+      </c>
+      <c r="C12" s="40">
+        <v>88.5</v>
+      </c>
+      <c r="D12" s="41">
+        <v>88</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41">
+        <v>0</v>
+      </c>
+      <c r="G12" s="40">
+        <v>0</v>
+      </c>
+      <c r="H12" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="46"/>
+      <c r="B13" s="41">
+        <f t="shared" ref="B13:D13" si="0">AVERAGE(B2:B12)</f>
+        <v>75.727272727272734</v>
+      </c>
+      <c r="C13" s="40">
+        <f t="shared" si="0"/>
+        <v>76.13636363636364</v>
+      </c>
+      <c r="D13" s="41">
+        <f t="shared" si="0"/>
+        <v>82.090909090909093</v>
+      </c>
+      <c r="E13" s="40"/>
+      <c r="F13" s="41">
+        <f t="shared" ref="F13:H13" si="1">AVERAGE(F2:F12)</f>
+        <v>2</v>
+      </c>
+      <c r="G13" s="40">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="46"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="41">
+        <v>66.5</v>
+      </c>
+      <c r="C15" s="40">
+        <v>79</v>
+      </c>
+      <c r="D15" s="41">
+        <v>75.5</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41">
+        <v>0</v>
+      </c>
+      <c r="G15" s="40">
+        <v>0</v>
+      </c>
+      <c r="H15" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="41">
+        <v>59</v>
+      </c>
+      <c r="C16" s="40">
+        <v>60.5</v>
+      </c>
+      <c r="D16" s="41">
+        <v>62.5</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41">
+        <v>0</v>
+      </c>
+      <c r="G16" s="40">
+        <v>0</v>
+      </c>
+      <c r="H16" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="39">
+        <v>39.5</v>
+      </c>
+      <c r="C17" s="45">
+        <v>44.5</v>
+      </c>
+      <c r="D17" s="41">
+        <v>72</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" s="41">
+        <v>21</v>
+      </c>
+      <c r="G17" s="40">
+        <v>12</v>
+      </c>
+      <c r="H17" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="41">
+        <v>82</v>
+      </c>
+      <c r="C18" s="40">
+        <v>80</v>
+      </c>
+      <c r="D18" s="41">
+        <v>81</v>
+      </c>
+      <c r="E18" s="40"/>
+      <c r="F18" s="41">
+        <v>0</v>
+      </c>
+      <c r="G18" s="40">
+        <v>0</v>
+      </c>
+      <c r="H18" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="41">
+        <v>66.5</v>
+      </c>
+      <c r="C19" s="40">
+        <v>77</v>
+      </c>
+      <c r="D19" s="41">
+        <v>75</v>
+      </c>
+      <c r="E19" s="40"/>
+      <c r="F19" s="41">
+        <v>0</v>
+      </c>
+      <c r="G19" s="40">
+        <v>0</v>
+      </c>
+      <c r="H19" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="39">
+        <v>48.5</v>
+      </c>
+      <c r="C20" s="45">
+        <v>55.5</v>
+      </c>
+      <c r="D20" s="41">
+        <v>59</v>
+      </c>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41">
+        <v>3.5</v>
+      </c>
+      <c r="G20" s="40">
+        <v>6.5</v>
+      </c>
+      <c r="H20" s="41">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="41">
+        <v>90.5</v>
+      </c>
+      <c r="C21" s="40">
+        <v>84</v>
+      </c>
+      <c r="D21" s="41">
+        <v>84</v>
+      </c>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41">
+        <v>0</v>
+      </c>
+      <c r="G21" s="40">
+        <v>0</v>
+      </c>
+      <c r="H21" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="41">
+        <v>67</v>
+      </c>
+      <c r="C22" s="40">
+        <v>79</v>
+      </c>
+      <c r="D22" s="41">
+        <v>79</v>
+      </c>
+      <c r="E22" s="40"/>
+      <c r="F22" s="41">
+        <v>0</v>
+      </c>
+      <c r="G22" s="40">
+        <v>0</v>
+      </c>
+      <c r="H22" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="39">
+        <v>46</v>
+      </c>
+      <c r="C23" s="40">
+        <v>66.5</v>
+      </c>
+      <c r="D23" s="41">
+        <v>72.5</v>
+      </c>
+      <c r="E23" s="40"/>
+      <c r="F23" s="41">
+        <v>5.5</v>
+      </c>
+      <c r="G23" s="40">
+        <v>0</v>
+      </c>
+      <c r="H23" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="41">
+        <v>75</v>
+      </c>
+      <c r="C24" s="40">
+        <v>79</v>
+      </c>
+      <c r="D24" s="41">
         <v>74.5</v>
       </c>
-      <c r="D3">
-        <v>72</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4">
-        <v>85</v>
-      </c>
-      <c r="C4">
-        <v>64.5</v>
-      </c>
-      <c r="D4" s="31">
-        <v>60</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>3.5</v>
-      </c>
-      <c r="H4">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5">
-        <v>83.5</v>
-      </c>
-      <c r="C5">
-        <v>84.5</v>
-      </c>
-      <c r="D5">
-        <v>85.5</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6">
-        <v>92</v>
-      </c>
-      <c r="C6">
-        <v>89</v>
-      </c>
-      <c r="D6">
-        <v>89</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="E24" s="40"/>
+      <c r="F24" s="41">
         <v>1</v>
       </c>
-      <c r="B7">
-        <v>82</v>
-      </c>
-      <c r="C7">
-        <v>66.5</v>
-      </c>
-      <c r="D7">
-        <v>63</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8">
-        <v>95</v>
-      </c>
-      <c r="C8">
-        <v>95</v>
-      </c>
-      <c r="D8">
-        <v>93.5</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>83</v>
-      </c>
-      <c r="C9">
-        <v>87</v>
-      </c>
-      <c r="D9">
-        <v>81.5</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>83</v>
-      </c>
-      <c r="C10">
-        <v>87</v>
-      </c>
-      <c r="D10">
-        <v>84.5</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11">
-        <v>88</v>
-      </c>
-      <c r="C11">
-        <v>87.5</v>
-      </c>
-      <c r="D11">
-        <v>85.5</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="G24" s="40">
+        <v>0</v>
+      </c>
+      <c r="H24" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B12">
-        <v>91</v>
-      </c>
-      <c r="C12">
-        <v>92</v>
-      </c>
-      <c r="D12">
-        <v>92</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <f t="shared" ref="B13" si="0">AVERAGE(B2:B12)</f>
-        <v>85.454545454545453</v>
-      </c>
-      <c r="C13">
-        <f t="shared" ref="C13" si="1">AVERAGE(C2:C12)</f>
-        <v>82.36363636363636</v>
-      </c>
-      <c r="D13">
-        <f>AVERAGE(D2:D12)</f>
-        <v>80.590909090909093</v>
-      </c>
-      <c r="F13">
-        <f t="shared" ref="E13:H13" si="2">AVERAGE(F2:F12)</f>
-        <v>0</v>
-      </c>
-      <c r="G13">
+      <c r="B25" s="41">
+        <v>81</v>
+      </c>
+      <c r="C25" s="40">
+        <v>82.5</v>
+      </c>
+      <c r="D25" s="41">
+        <v>80.5</v>
+      </c>
+      <c r="E25" s="40"/>
+      <c r="F25" s="41">
+        <v>0</v>
+      </c>
+      <c r="G25" s="40">
+        <v>0</v>
+      </c>
+      <c r="H25" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="46"/>
+      <c r="B26" s="41">
+        <f t="shared" ref="B26:D26" si="2">AVERAGE(B15:B25)</f>
+        <v>65.590909090909093</v>
+      </c>
+      <c r="C26" s="40">
         <f t="shared" si="2"/>
-        <v>0.31818181818181818</v>
-      </c>
-      <c r="H13">
+        <v>71.590909090909093</v>
+      </c>
+      <c r="D26" s="41">
         <f t="shared" si="2"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15">
-        <v>82.5</v>
-      </c>
-      <c r="C15">
-        <v>80</v>
-      </c>
-      <c r="D15">
-        <v>82.5</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" s="19">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>64</v>
-      </c>
-      <c r="C16">
-        <v>62.5</v>
-      </c>
-      <c r="D16">
-        <v>64</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16" s="18">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17">
-        <v>80</v>
-      </c>
-      <c r="C17">
-        <v>80</v>
-      </c>
-      <c r="D17">
-        <v>60</v>
-      </c>
-      <c r="F17">
-        <v>0.5</v>
-      </c>
-      <c r="G17" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="H17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18">
-        <v>83</v>
-      </c>
-      <c r="C18">
-        <v>81</v>
-      </c>
-      <c r="D18">
-        <v>84</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18" s="18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19">
-        <v>84</v>
-      </c>
-      <c r="C19">
-        <v>78.5</v>
-      </c>
-      <c r="D19">
-        <v>78.5</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19" s="18">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20">
-        <v>70.5</v>
-      </c>
-      <c r="C20">
-        <v>54.5</v>
-      </c>
-      <c r="D20">
-        <v>54</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="18">
-        <v>6.5</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21">
-        <v>90</v>
-      </c>
-      <c r="C21">
-        <v>91.5</v>
-      </c>
-      <c r="D21">
-        <v>92</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" s="18">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22">
-        <v>82</v>
-      </c>
-      <c r="C22">
-        <v>81.5</v>
-      </c>
-      <c r="D22">
-        <v>70.5</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22" s="18">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23">
-        <v>82</v>
-      </c>
-      <c r="C23">
-        <v>73</v>
-      </c>
-      <c r="D23">
-        <v>67</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23" s="18">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24">
-        <v>86.5</v>
-      </c>
-      <c r="C24">
-        <v>81.5</v>
-      </c>
-      <c r="D24">
-        <v>82</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24" s="18">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25">
-        <v>84</v>
-      </c>
-      <c r="C25">
-        <v>83.5</v>
-      </c>
-      <c r="D25">
-        <v>85</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25" s="18">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <f t="shared" ref="B26:D26" si="3">AVERAGE(B15:B25)</f>
-        <v>80.772727272727266</v>
-      </c>
-      <c r="C26">
-        <f>AVERAGE(C15:C25)</f>
-        <v>77.045454545454547</v>
-      </c>
-      <c r="D26">
-        <f>AVERAGE(D15:D25)</f>
-        <v>74.5</v>
-      </c>
-      <c r="F26">
-        <f t="shared" ref="E26:H26" si="4">AVERAGE(F15:F25)</f>
-        <v>4.5454545454545456E-2</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="4"/>
-        <v>0.72727272727272729</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="4"/>
-        <v>2.6818181818181817</v>
+        <v>74.13636363636364</v>
+      </c>
+      <c r="E26" s="40"/>
+      <c r="F26" s="41">
+        <f t="shared" ref="F26:H26" si="3">AVERAGE(F15:F25)</f>
+        <v>2.8181818181818183</v>
+      </c>
+      <c r="G26" s="40">
+        <f t="shared" si="3"/>
+        <v>1.6818181818181819</v>
+      </c>
+      <c r="H26" s="41">
+        <f t="shared" si="3"/>
+        <v>0.13636363636363635</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>